<commit_message>
Finalisation des spécifications de l'application
Ajout des chapitre. modification .ignore, modification diagramme
</commit_message>
<xml_diff>
--- a/Documentation/HoferL-JournalPlanif-M5.xlsx
+++ b/Documentation/HoferL-JournalPlanif-M5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" state="visible" r:id="rId1"/>
@@ -377,7 +377,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="65">
+  <borders count="66">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -395,16 +395,18 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color theme="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
+      <top style="thin">
+        <color theme="1"/>
       </top>
-      <bottom style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal style="none"/>
     </border>
     <border>
@@ -436,6 +438,19 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
@@ -1140,7 +1155,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,19 +1208,19 @@
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="180" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -1220,13 +1235,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="15" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,8 +1250,11 @@
     <xf fontId="0" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1244,9 +1262,6 @@
     </xf>
     <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1257,117 +1272,120 @@
     <xf fontId="0" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="29" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="29" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="29" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="30" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="31" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="31" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="31" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="32" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="33" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="33" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="34" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="32" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="5" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="33" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="5" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="37" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="38" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="38" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="39" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="39" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="40" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="40" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="41" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="41" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="42" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="43" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="44" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="44" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="45" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="45" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="46" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="46" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="47" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="48" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="49" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="47" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="50" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="51" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="48" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="51" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="52" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="53" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="29" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="48" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="54" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="49" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="54" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="50" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="55" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="56" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="57" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="58" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="58" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="59" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="59" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="60" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="60" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="61" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="61" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="62" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="63" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="64" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="65" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4277,7 +4295,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>4.1666666666666664e-002</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
@@ -4294,7 +4312,7 @@
       </c>
       <c r="I4" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>4.5454545454545456e-002</v>
+        <v>0.045454545454545456</v>
       </c>
     </row>
     <row r="5" ht="28.800000000000001">
@@ -4327,7 +4345,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="4">
-        <v>4.1666666666666664e-002</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -4352,7 +4370,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="4">
-        <v>4.1666666666666664e-002</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -4427,7 +4445,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4">
-        <v>8.3333333333333329e-002</v>
+        <v>0.083333333333333329</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -4452,7 +4470,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="4">
-        <v>4.1666666666666664e-002</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>12</v>
@@ -4473,7 +4491,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="4">
-        <v>4.1666666666666664e-002</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>10</v>
@@ -4488,7 +4506,7 @@
         <v>46056</v>
       </c>
       <c r="C13" s="4">
-        <v>8.3333333333333329e-002</v>
+        <v>0.083333333333333329</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>12</v>
@@ -4904,7 +4922,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="1">
-        <x14:dataValidation xr:uid="{008B0079-00F2-4CD0-920D-0023008800FD}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{003A0099-00CB-4CC4-B95E-004500930027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$G$3:$G$7</xm:f>
           </x14:formula1>
@@ -6505,7 +6523,7 @@
       <selection activeCell="AD2" activeCellId="0" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="3" max="3" width="31.33203125"/>
     <col customWidth="1" min="5" max="49" width="3.44140625"/>
@@ -6557,7 +6575,7 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" ht="98.549999999999997" customHeight="1">
+    <row r="2" ht="106.2" customHeight="1">
       <c r="B2" s="19" t="s">
         <v>35</v>
       </c>
@@ -6690,12 +6708,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="AF1:AJ1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="O1:V1"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -6739,85 +6757,85 @@
       <c r="C2" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36" t="s">
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="36" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="36" t="s">
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="37"/>
-      <c r="AD2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="AD2" s="39"/>
     </row>
     <row r="3">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="43">
         <v>4</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="44">
         <v>1</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="45">
         <v>2</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="45">
         <v>3</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="43">
         <v>4</v>
       </c>
-      <c r="J3" s="43">
+      <c r="J3" s="44">
         <v>1</v>
       </c>
-      <c r="K3" s="44">
+      <c r="K3" s="45">
         <v>2</v>
       </c>
-      <c r="L3" s="44">
+      <c r="L3" s="45">
         <v>3</v>
       </c>
-      <c r="M3" s="42">
+      <c r="M3" s="43">
         <v>4</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="44">
         <v>1</v>
       </c>
-      <c r="O3" s="44">
+      <c r="O3" s="45">
         <v>2</v>
       </c>
-      <c r="P3" s="44">
+      <c r="P3" s="45">
         <v>3</v>
       </c>
-      <c r="Q3" s="42">
+      <c r="Q3" s="43">
         <v>4</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="44">
         <v>1</v>
       </c>
-      <c r="S3" s="45">
+      <c r="S3" s="46">
         <v>2</v>
       </c>
       <c r="U3" t="s">
@@ -6825,187 +6843,187 @@
       </c>
     </row>
     <row r="4" ht="12" customHeight="1">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="52"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="53"/>
       <c r="U4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" ht="12" customHeight="1">
-      <c r="B5" s="46"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="60"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="61"/>
     </row>
     <row r="6" ht="12" customHeight="1">
-      <c r="B6" s="46"/>
-      <c r="C6" s="61" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="67"/>
-      <c r="S6" s="68"/>
-      <c r="U6" s="69" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="69"/>
+      <c r="U6" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="V6" s="69"/>
+      <c r="V6" s="70"/>
     </row>
     <row r="7" ht="12" customHeight="1">
-      <c r="B7" s="46"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="60"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="61"/>
       <c r="U7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1">
-      <c r="B8" s="46"/>
-      <c r="C8" s="61" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="67"/>
-      <c r="S8" s="68"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="69"/>
       <c r="U8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" ht="12" customHeight="1">
-      <c r="B9" s="46"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="55"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="60"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="61"/>
     </row>
     <row r="10" ht="12" customHeight="1">
-      <c r="B10" s="46"/>
-      <c r="C10" s="61" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="68"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="67"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="69"/>
     </row>
     <row r="11" ht="12" customHeight="1">
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="77"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="75"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="78"/>
     </row>
     <row r="12" ht="12" customHeight="1">
       <c r="B12" s="33" t="s">
@@ -7014,516 +7032,516 @@
       <c r="C12" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="52"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="53"/>
     </row>
     <row r="13" ht="12" customHeight="1">
-      <c r="B13" s="46"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="60"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="61"/>
     </row>
     <row r="14" ht="12" customHeight="1">
-      <c r="B14" s="46"/>
-      <c r="C14" s="61" t="s">
+      <c r="B14" s="47"/>
+      <c r="C14" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="67"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="66"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="68"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="67"/>
+      <c r="P14" s="67"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="69"/>
     </row>
     <row r="15" ht="12" customHeight="1">
-      <c r="B15" s="46"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="60"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="61"/>
     </row>
     <row r="16" ht="12" customHeight="1">
-      <c r="B16" s="46"/>
-      <c r="C16" s="61" t="s">
+      <c r="B16" s="47"/>
+      <c r="C16" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="67"/>
-      <c r="S16" s="68"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="83"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="64"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="69"/>
     </row>
     <row r="17" ht="12" customHeight="1">
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="83"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="77"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="76"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="78"/>
     </row>
     <row r="18" ht="12" customHeight="1">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="35" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="52"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="53"/>
     </row>
     <row r="19" ht="12" customHeight="1">
-      <c r="B19" s="46"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="58"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="60"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="61"/>
     </row>
     <row r="20" ht="12" customHeight="1">
-      <c r="B20" s="46"/>
-      <c r="C20" s="61" t="s">
+      <c r="B20" s="47"/>
+      <c r="C20" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="67"/>
-      <c r="O20" s="66"/>
-      <c r="P20" s="66"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="67"/>
-      <c r="S20" s="68"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="83"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="64"/>
+      <c r="R20" s="68"/>
+      <c r="S20" s="69"/>
     </row>
     <row r="21" ht="12" customHeight="1">
-      <c r="B21" s="46"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="58"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="84"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="55"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="60"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="61"/>
     </row>
     <row r="22" ht="12" customHeight="1">
-      <c r="B22" s="46"/>
-      <c r="C22" s="61" t="s">
+      <c r="B22" s="47"/>
+      <c r="C22" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="63"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="68"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="68"/>
+      <c r="S22" s="69"/>
     </row>
     <row r="23" ht="12" customHeight="1">
-      <c r="B23" s="70"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="74"/>
-      <c r="S23" s="77"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="75"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="75"/>
+      <c r="S23" s="78"/>
     </row>
     <row r="24" ht="12" customHeight="1">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="35" t="s">
         <v>89</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="79"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="78"/>
-      <c r="P24" s="78"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="52"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="53"/>
     </row>
     <row r="25" ht="12" customHeight="1">
-      <c r="B25" s="46"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="60"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="61"/>
     </row>
     <row r="26" ht="12" customHeight="1">
-      <c r="B26" s="46"/>
-      <c r="C26" s="61" t="s">
+      <c r="B26" s="47"/>
+      <c r="C26" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="63"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="66"/>
-      <c r="L26" s="66"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="68"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="64"/>
+      <c r="R26" s="68"/>
+      <c r="S26" s="69"/>
     </row>
     <row r="27" ht="12" customHeight="1">
-      <c r="B27" s="46"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="60"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="61"/>
     </row>
     <row r="28" ht="12" customHeight="1">
-      <c r="B28" s="46"/>
-      <c r="C28" s="61" t="s">
+      <c r="B28" s="47"/>
+      <c r="C28" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="66"/>
-      <c r="M28" s="63"/>
-      <c r="N28" s="67"/>
-      <c r="O28" s="66"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="82"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="68"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="67"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="83"/>
+      <c r="R28" s="68"/>
+      <c r="S28" s="69"/>
     </row>
     <row r="29" ht="12" customHeight="1">
-      <c r="B29" s="46"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="88"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="88"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="86"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="89"/>
-      <c r="P29" s="88"/>
-      <c r="Q29" s="86"/>
-      <c r="R29" s="87"/>
-      <c r="S29" s="91"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="88"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="88"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="87"/>
+      <c r="R29" s="88"/>
+      <c r="S29" s="92"/>
     </row>
     <row r="30" ht="12" customHeight="1">
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="93" t="s">
+      <c r="C30" s="94" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="97"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="97"/>
-      <c r="N30" s="95"/>
-      <c r="O30" s="96"/>
-      <c r="P30" s="95"/>
-      <c r="Q30" s="97"/>
-      <c r="R30" s="95"/>
-      <c r="S30" s="98"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="96"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="97"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="96"/>
+      <c r="O30" s="97"/>
+      <c r="P30" s="96"/>
+      <c r="Q30" s="98"/>
+      <c r="R30" s="96"/>
+      <c r="S30" s="99"/>
     </row>
     <row r="31" ht="12" customHeight="1">
-      <c r="B31" s="99"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="102"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="104"/>
-      <c r="N31" s="102"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="102"/>
-      <c r="Q31" s="104"/>
-      <c r="R31" s="102"/>
-      <c r="S31" s="60"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="105"/>
+      <c r="J31" s="103"/>
+      <c r="K31" s="106"/>
+      <c r="L31" s="104"/>
+      <c r="M31" s="105"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="104"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="105"/>
+      <c r="R31" s="103"/>
+      <c r="S31" s="61"/>
     </row>
     <row r="32" ht="12" customHeight="1">
-      <c r="B32" s="99"/>
-      <c r="C32" s="100" t="s">
+      <c r="B32" s="100"/>
+      <c r="C32" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="107"/>
-      <c r="G32" s="107"/>
-      <c r="H32" s="108"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="107"/>
-      <c r="K32" s="107"/>
-      <c r="L32" s="108"/>
-      <c r="M32" s="109"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="108"/>
-      <c r="P32" s="107"/>
-      <c r="Q32" s="109"/>
-      <c r="R32" s="107"/>
-      <c r="S32" s="110"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="107"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="108"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="108"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="111"/>
     </row>
     <row r="33" ht="12" customHeight="1">
-      <c r="B33" s="99"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="111"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="102"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="103"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="102"/>
-      <c r="O33" s="103"/>
-      <c r="P33" s="102"/>
-      <c r="Q33" s="104"/>
-      <c r="R33" s="102"/>
-      <c r="S33" s="60"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="112"/>
+      <c r="I33" s="113"/>
+      <c r="J33" s="103"/>
+      <c r="K33" s="106"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="105"/>
+      <c r="N33" s="103"/>
+      <c r="O33" s="104"/>
+      <c r="P33" s="103"/>
+      <c r="Q33" s="105"/>
+      <c r="R33" s="103"/>
+      <c r="S33" s="61"/>
     </row>
     <row r="34" ht="12" customHeight="1">
-      <c r="B34" s="99"/>
-      <c r="C34" s="53" t="s">
+      <c r="B34" s="100"/>
+      <c r="C34" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="114"/>
-      <c r="K34" s="114"/>
-      <c r="L34" s="115"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="114"/>
-      <c r="O34" s="115"/>
-      <c r="P34" s="114"/>
-      <c r="Q34" s="116"/>
-      <c r="R34" s="114"/>
-      <c r="S34" s="117"/>
-      <c r="U34" s="118"/>
-      <c r="V34" s="119" t="s">
+      <c r="D34" s="86"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="115"/>
+      <c r="K34" s="115"/>
+      <c r="L34" s="116"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="115"/>
+      <c r="O34" s="116"/>
+      <c r="P34" s="115"/>
+      <c r="Q34" s="117"/>
+      <c r="R34" s="115"/>
+      <c r="S34" s="118"/>
+      <c r="U34" s="119"/>
+      <c r="V34" s="120" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="35" ht="13.800000000000001" customHeight="1">
-      <c r="B35" s="120"/>
-      <c r="C35" s="121"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="122"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="123"/>
-      <c r="H35" s="124"/>
-      <c r="I35" s="125"/>
-      <c r="J35" s="123"/>
-      <c r="K35" s="123"/>
-      <c r="L35" s="124"/>
-      <c r="M35" s="125"/>
-      <c r="N35" s="123"/>
-      <c r="O35" s="124"/>
-      <c r="P35" s="123"/>
-      <c r="Q35" s="125"/>
-      <c r="R35" s="123"/>
-      <c r="S35" s="77"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="126"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="125"/>
+      <c r="M35" s="126"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="125"/>
+      <c r="P35" s="124"/>
+      <c r="Q35" s="126"/>
+      <c r="R35" s="124"/>
+      <c r="S35" s="78"/>
       <c r="U35" s="31"/>
-      <c r="V35" s="126" t="s">
+      <c r="V35" s="127" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout chapitre Diagramme de classe
Ajout de description, diagramme, légère correction dans .drawio
</commit_message>
<xml_diff>
--- a/Documentation/HoferL-JournalPlanif-M5.xlsx
+++ b/Documentation/HoferL-JournalPlanif-M5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>date</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t xml:space="preserve">Révision de la licence et des citation des ressources GPL3.0-Only parce que l'opensource c'est génial. Ajout du chapitre public cible dans la documentation technique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commencement de la documentation sur l'exigence de l'application.</t>
+  </si>
+  <si>
+    <t>04.02.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de diagrammes (cas utilisation, MCD, classe), mis en pause, analyse pas terminé.</t>
+  </si>
+  <si>
+    <t>05.02.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation de la documentation analyse de l'application. </t>
   </si>
   <si>
     <t>Janvier</t>
@@ -1155,7 +1170,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1190,6 +1205,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="167" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -3719,8 +3743,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Journal" ref="B2:E13">
-  <autoFilter ref="B2:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Journal" ref="B2:E16">
+  <autoFilter ref="B2:E16"/>
   <tableColumns count="4">
     <tableColumn id="1" name="date" dataDxfId="0"/>
     <tableColumn id="2" name="Temps" dataDxfId="1"/>
@@ -4517,22 +4541,46 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14">
-      <c r="B14" s="13"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="13">
+        <v>46057</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.083333333333333329</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16">
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="3"/>
@@ -4922,7 +4970,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="1">
-        <x14:dataValidation xr:uid="{003A0099-00CB-4CC4-B95E-004500930027}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000A003D-0045-4696-AF39-006300EB0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$G$3:$G$7</xm:f>
           </x14:formula1>
@@ -4943,7 +4991,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="14" width="5.6640625"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="17" width="5.6640625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" width="12.21875"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="9.5546875"/>
     <col bestFit="1" customWidth="1" min="6" max="6" width="11.109375"/>
@@ -4959,55 +5007,55 @@
       <c r="C1"/>
     </row>
     <row r="2">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="18" t="str">
         <f t="array" ref="A2:A6">_xlfn.UNIQUE(Journal[date])</f>
         <v>20.01.2026</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="19">
         <f>SUMIF(Journal[date],SommeParJours!A2,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C2" s="16"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="str">
+      <c r="A3" s="18" t="str">
         <f/>
         <v>27.01.2026</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="19">
         <f>SUMIF(Journal[date],SommeParJours!A3,Journal[Temps])</f>
         <v>0.20833333333333331</v>
       </c>
       <c r="C3"/>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="str">
+      <c r="A4" s="18" t="str">
         <f/>
         <v>30.01.2026</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="19">
         <f>SUMIF(Journal[date],SommeParJours!A4,Journal[Temps])</f>
         <v>0.29166666666666663</v>
       </c>
       <c r="C4"/>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="str">
+      <c r="A5" s="18" t="str">
         <f/>
         <v>03.02.2026</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="19">
         <f>SUMIF(Journal[date],SommeParJours!A5,Journal[Temps])</f>
         <v>0.25</v>
       </c>
       <c r="C5"/>
     </row>
     <row r="6">
-      <c r="A6" s="15">
+      <c r="A6" s="18">
         <f/>
         <v>46056</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="19">
         <f>SUMIF(Journal[date],SommeParJours!A6,Journal[Temps])</f>
         <v>0.25</v>
       </c>
@@ -5071,1441 +5119,1441 @@
       <c r="C25"/>
     </row>
     <row r="26">
-      <c r="C26" s="17">
+      <c r="C26" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A26,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="17">
+      <c r="C27" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A27,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="17">
+      <c r="C28" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A28,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="17">
+      <c r="C29" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A29,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="17">
+      <c r="C30" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A30,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="17">
+      <c r="C31" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A31,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="17">
+      <c r="C32" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A32,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="17">
+      <c r="C33" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A33,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="17">
+      <c r="C34" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A34,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="C35" s="17">
+      <c r="C35" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A35,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="17">
+      <c r="C36" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A36,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="17">
+      <c r="C37" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A37,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="17">
+      <c r="C38" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A38,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="17">
+      <c r="C39" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A39,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="18"/>
-      <c r="B40" s="16" t="str">
+      <c r="A40" s="21"/>
+      <c r="B40" s="19" t="str">
         <f t="shared" ref="B40:B103" si="0">IF(C40&gt;0,C40,"")</f>
         <v/>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A40,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="18"/>
-      <c r="B41" s="16" t="str">
+      <c r="A41" s="21"/>
+      <c r="B41" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A41,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="18"/>
-      <c r="B42" s="16" t="str">
+      <c r="A42" s="21"/>
+      <c r="B42" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A42,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="18"/>
-      <c r="B43" s="16" t="str">
+      <c r="A43" s="21"/>
+      <c r="B43" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A43,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="18"/>
-      <c r="B44" s="16" t="str">
+      <c r="A44" s="21"/>
+      <c r="B44" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A44,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="18"/>
-      <c r="B45" s="16" t="str">
+      <c r="A45" s="21"/>
+      <c r="B45" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A45,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="18"/>
-      <c r="B46" s="16" t="str">
+      <c r="A46" s="21"/>
+      <c r="B46" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A46,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="18"/>
-      <c r="B47" s="16" t="str">
+      <c r="A47" s="21"/>
+      <c r="B47" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A47,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="18"/>
-      <c r="B48" s="16" t="str">
+      <c r="A48" s="21"/>
+      <c r="B48" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A48,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="18"/>
-      <c r="B49" s="16" t="str">
+      <c r="A49" s="21"/>
+      <c r="B49" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A49,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="18"/>
-      <c r="B50" s="16" t="str">
+      <c r="A50" s="21"/>
+      <c r="B50" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C50" s="17">
+      <c r="C50" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A50,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="18"/>
-      <c r="B51" s="16" t="str">
+      <c r="A51" s="21"/>
+      <c r="B51" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A51,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="18"/>
-      <c r="B52" s="16" t="str">
+      <c r="A52" s="21"/>
+      <c r="B52" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A52,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="18"/>
-      <c r="B53" s="16" t="str">
+      <c r="A53" s="21"/>
+      <c r="B53" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C53" s="17">
+      <c r="C53" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A53,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="18"/>
-      <c r="B54" s="16" t="str">
+      <c r="A54" s="21"/>
+      <c r="B54" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C54" s="17">
+      <c r="C54" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A54,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="18"/>
-      <c r="B55" s="16" t="str">
+      <c r="A55" s="21"/>
+      <c r="B55" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C55" s="17">
+      <c r="C55" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A55,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="18"/>
-      <c r="B56" s="16" t="str">
+      <c r="A56" s="21"/>
+      <c r="B56" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C56" s="17">
+      <c r="C56" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A56,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="18"/>
-      <c r="B57" s="16" t="str">
+      <c r="A57" s="21"/>
+      <c r="B57" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A57,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="18"/>
-      <c r="B58" s="16" t="str">
+      <c r="A58" s="21"/>
+      <c r="B58" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A58,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="18"/>
-      <c r="B59" s="16" t="str">
+      <c r="A59" s="21"/>
+      <c r="B59" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C59" s="17">
+      <c r="C59" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A59,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="18"/>
-      <c r="B60" s="16" t="str">
+      <c r="A60" s="21"/>
+      <c r="B60" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C60" s="17">
+      <c r="C60" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A60,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="18"/>
-      <c r="B61" s="16" t="str">
+      <c r="A61" s="21"/>
+      <c r="B61" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C61" s="17">
+      <c r="C61" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A61,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="18"/>
-      <c r="B62" s="16" t="str">
+      <c r="A62" s="21"/>
+      <c r="B62" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C62" s="17">
+      <c r="C62" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A62,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="18"/>
-      <c r="B63" s="16" t="str">
+      <c r="A63" s="21"/>
+      <c r="B63" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A63,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="18"/>
-      <c r="B64" s="16" t="str">
+      <c r="A64" s="21"/>
+      <c r="B64" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A64,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="18"/>
-      <c r="B65" s="16" t="str">
+      <c r="A65" s="21"/>
+      <c r="B65" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A65,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="18"/>
-      <c r="B66" s="16" t="str">
+      <c r="A66" s="21"/>
+      <c r="B66" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A66,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="18"/>
-      <c r="B67" s="16" t="str">
+      <c r="A67" s="21"/>
+      <c r="B67" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C67" s="17">
+      <c r="C67" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A67,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="18"/>
-      <c r="B68" s="16" t="str">
+      <c r="A68" s="21"/>
+      <c r="B68" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A68,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="18"/>
-      <c r="B69" s="16" t="str">
+      <c r="A69" s="21"/>
+      <c r="B69" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A69,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="18"/>
-      <c r="B70" s="16" t="str">
+      <c r="A70" s="21"/>
+      <c r="B70" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C70" s="17">
+      <c r="C70" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A70,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="18"/>
-      <c r="B71" s="16" t="str">
+      <c r="A71" s="21"/>
+      <c r="B71" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C71" s="17">
+      <c r="C71" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A71,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="18"/>
-      <c r="B72" s="16" t="str">
+      <c r="A72" s="21"/>
+      <c r="B72" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C72" s="17">
+      <c r="C72" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A72,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="18"/>
-      <c r="B73" s="16" t="str">
+      <c r="A73" s="21"/>
+      <c r="B73" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C73" s="17">
+      <c r="C73" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A73,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="18"/>
-      <c r="B74" s="16" t="str">
+      <c r="A74" s="21"/>
+      <c r="B74" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C74" s="17">
+      <c r="C74" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A74,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="18"/>
-      <c r="B75" s="16" t="str">
+      <c r="A75" s="21"/>
+      <c r="B75" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C75" s="17">
+      <c r="C75" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A75,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="18"/>
-      <c r="B76" s="16" t="str">
+      <c r="A76" s="21"/>
+      <c r="B76" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C76" s="17">
+      <c r="C76" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A76,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="18"/>
-      <c r="B77" s="16" t="str">
+      <c r="A77" s="21"/>
+      <c r="B77" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C77" s="17">
+      <c r="C77" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A77,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="18"/>
-      <c r="B78" s="16" t="str">
+      <c r="A78" s="21"/>
+      <c r="B78" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C78" s="17">
+      <c r="C78" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A78,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="18"/>
-      <c r="B79" s="16" t="str">
+      <c r="A79" s="21"/>
+      <c r="B79" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C79" s="17">
+      <c r="C79" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A79,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="18"/>
-      <c r="B80" s="16" t="str">
+      <c r="A80" s="21"/>
+      <c r="B80" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C80" s="17">
+      <c r="C80" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A80,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="18"/>
-      <c r="B81" s="16" t="str">
+      <c r="A81" s="21"/>
+      <c r="B81" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C81" s="17">
+      <c r="C81" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A81,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="18"/>
-      <c r="B82" s="16" t="str">
+      <c r="A82" s="21"/>
+      <c r="B82" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C82" s="17">
+      <c r="C82" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A82,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="18"/>
-      <c r="B83" s="16" t="str">
+      <c r="A83" s="21"/>
+      <c r="B83" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C83" s="17">
+      <c r="C83" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A83,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="18"/>
-      <c r="B84" s="16" t="str">
+      <c r="A84" s="21"/>
+      <c r="B84" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C84" s="17">
+      <c r="C84" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A84,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="18"/>
-      <c r="B85" s="16" t="str">
+      <c r="A85" s="21"/>
+      <c r="B85" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C85" s="17">
+      <c r="C85" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A85,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="18"/>
-      <c r="B86" s="16" t="str">
+      <c r="A86" s="21"/>
+      <c r="B86" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C86" s="17">
+      <c r="C86" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A86,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="18"/>
-      <c r="B87" s="16" t="str">
+      <c r="A87" s="21"/>
+      <c r="B87" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C87" s="17">
+      <c r="C87" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A87,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="18"/>
-      <c r="B88" s="16" t="str">
+      <c r="A88" s="21"/>
+      <c r="B88" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C88" s="17">
+      <c r="C88" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A88,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="18"/>
-      <c r="B89" s="16" t="str">
+      <c r="A89" s="21"/>
+      <c r="B89" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C89" s="17">
+      <c r="C89" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A89,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="18"/>
-      <c r="B90" s="16" t="str">
+      <c r="A90" s="21"/>
+      <c r="B90" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C90" s="17">
+      <c r="C90" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A90,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="18"/>
-      <c r="B91" s="16" t="str">
+      <c r="A91" s="21"/>
+      <c r="B91" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C91" s="17">
+      <c r="C91" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A91,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="18"/>
-      <c r="B92" s="16" t="str">
+      <c r="A92" s="21"/>
+      <c r="B92" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C92" s="17">
+      <c r="C92" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A92,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="18"/>
-      <c r="B93" s="16" t="str">
+      <c r="A93" s="21"/>
+      <c r="B93" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C93" s="17">
+      <c r="C93" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A93,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="18"/>
-      <c r="B94" s="16" t="str">
+      <c r="A94" s="21"/>
+      <c r="B94" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C94" s="17">
+      <c r="C94" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A94,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="18"/>
-      <c r="B95" s="16" t="str">
+      <c r="A95" s="21"/>
+      <c r="B95" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C95" s="17">
+      <c r="C95" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A95,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="18"/>
-      <c r="B96" s="16" t="str">
+      <c r="A96" s="21"/>
+      <c r="B96" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C96" s="17">
+      <c r="C96" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A96,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="18"/>
-      <c r="B97" s="16" t="str">
+      <c r="A97" s="21"/>
+      <c r="B97" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C97" s="17">
+      <c r="C97" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A97,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="18"/>
-      <c r="B98" s="16" t="str">
+      <c r="A98" s="21"/>
+      <c r="B98" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C98" s="17">
+      <c r="C98" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A98,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="18"/>
-      <c r="B99" s="16" t="str">
+      <c r="A99" s="21"/>
+      <c r="B99" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C99" s="17">
+      <c r="C99" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A99,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="18"/>
-      <c r="B100" s="16" t="str">
+      <c r="A100" s="21"/>
+      <c r="B100" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C100" s="17">
+      <c r="C100" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A100,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="18"/>
-      <c r="B101" s="16" t="str">
+      <c r="A101" s="21"/>
+      <c r="B101" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C101" s="17">
+      <c r="C101" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A101,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="18"/>
-      <c r="B102" s="16" t="str">
+      <c r="A102" s="21"/>
+      <c r="B102" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C102" s="17">
+      <c r="C102" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A102,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="18"/>
-      <c r="B103" s="16" t="str">
+      <c r="A103" s="21"/>
+      <c r="B103" s="19" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C103" s="17">
+      <c r="C103" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A103,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="18"/>
-      <c r="B104" s="16" t="str">
+      <c r="A104" s="21"/>
+      <c r="B104" s="19" t="str">
         <f t="shared" ref="B104:B114" si="1">IF(C104&gt;0,C104,"")</f>
         <v/>
       </c>
-      <c r="C104" s="17">
+      <c r="C104" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A104,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="18"/>
-      <c r="B105" s="16" t="str">
+      <c r="A105" s="21"/>
+      <c r="B105" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C105" s="17">
+      <c r="C105" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A105,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="18"/>
-      <c r="B106" s="16" t="str">
+      <c r="A106" s="21"/>
+      <c r="B106" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C106" s="17">
+      <c r="C106" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A106,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="18"/>
-      <c r="B107" s="16" t="str">
+      <c r="A107" s="21"/>
+      <c r="B107" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C107" s="17">
+      <c r="C107" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A107,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="18"/>
-      <c r="B108" s="16" t="str">
+      <c r="A108" s="21"/>
+      <c r="B108" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C108" s="17">
+      <c r="C108" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A108,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="18"/>
-      <c r="B109" s="16" t="str">
+      <c r="A109" s="21"/>
+      <c r="B109" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C109" s="17">
+      <c r="C109" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A109,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="18"/>
-      <c r="B110" s="16" t="str">
+      <c r="A110" s="21"/>
+      <c r="B110" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C110" s="17">
+      <c r="C110" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A110,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="18"/>
-      <c r="B111" s="16" t="str">
+      <c r="A111" s="21"/>
+      <c r="B111" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C111" s="17">
+      <c r="C111" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A111,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="18"/>
-      <c r="B112" s="16" t="str">
+      <c r="A112" s="21"/>
+      <c r="B112" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C112" s="17">
+      <c r="C112" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A112,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="18"/>
-      <c r="B113" s="16" t="str">
+      <c r="A113" s="21"/>
+      <c r="B113" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C113" s="17">
+      <c r="C113" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A113,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="18"/>
-      <c r="B114" s="16" t="str">
+      <c r="A114" s="21"/>
+      <c r="B114" s="19" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C114" s="17">
+      <c r="C114" s="20">
         <f>SUMIF(Journal[date],SommeParJours!A114,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="18"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="17"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="20"/>
     </row>
     <row r="116">
-      <c r="A116" s="18"/>
-      <c r="B116" s="18"/>
-      <c r="C116" s="17"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="20"/>
     </row>
     <row r="117">
-      <c r="A117" s="18"/>
-      <c r="B117" s="18"/>
-      <c r="C117" s="17"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="20"/>
     </row>
     <row r="118">
-      <c r="A118" s="18"/>
-      <c r="B118" s="18"/>
-      <c r="C118" s="17"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="20"/>
     </row>
     <row r="119">
-      <c r="A119" s="18"/>
-      <c r="B119" s="18"/>
-      <c r="C119" s="17"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="20"/>
     </row>
     <row r="120">
-      <c r="A120" s="18"/>
-      <c r="B120" s="18"/>
-      <c r="C120" s="17"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="20"/>
     </row>
     <row r="121">
-      <c r="A121" s="18"/>
-      <c r="B121" s="18"/>
-      <c r="C121" s="17"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="20"/>
     </row>
     <row r="122">
-      <c r="A122" s="18"/>
-      <c r="B122" s="18"/>
-      <c r="C122" s="17"/>
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="20"/>
     </row>
     <row r="123">
-      <c r="A123" s="18"/>
-      <c r="B123" s="18"/>
-      <c r="C123" s="17"/>
+      <c r="A123" s="21"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="20"/>
     </row>
     <row r="124">
-      <c r="A124" s="18"/>
-      <c r="B124" s="18"/>
-      <c r="C124" s="17"/>
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="20"/>
     </row>
     <row r="125">
-      <c r="A125" s="18"/>
-      <c r="B125" s="18"/>
-      <c r="C125" s="17"/>
+      <c r="A125" s="21"/>
+      <c r="B125" s="21"/>
+      <c r="C125" s="20"/>
     </row>
     <row r="126">
-      <c r="A126" s="18"/>
-      <c r="B126" s="18"/>
-      <c r="C126" s="17"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="20"/>
     </row>
     <row r="127">
-      <c r="A127" s="18"/>
-      <c r="B127" s="18"/>
-      <c r="C127" s="17"/>
+      <c r="A127" s="21"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="20"/>
     </row>
     <row r="128">
-      <c r="A128" s="18"/>
-      <c r="B128" s="18"/>
-      <c r="C128" s="17"/>
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="20"/>
     </row>
     <row r="129">
-      <c r="A129" s="18"/>
-      <c r="B129" s="18"/>
-      <c r="C129" s="17"/>
+      <c r="A129" s="21"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="20"/>
     </row>
     <row r="130">
-      <c r="A130" s="18"/>
-      <c r="B130" s="18"/>
-      <c r="C130" s="17"/>
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="20"/>
     </row>
     <row r="131">
-      <c r="A131" s="18"/>
-      <c r="B131" s="18"/>
-      <c r="C131" s="17"/>
+      <c r="A131" s="21"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="20"/>
     </row>
     <row r="132">
-      <c r="A132" s="18"/>
-      <c r="B132" s="18"/>
-      <c r="C132" s="17"/>
+      <c r="A132" s="21"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="20"/>
     </row>
     <row r="133">
-      <c r="A133" s="18"/>
-      <c r="B133" s="18"/>
-      <c r="C133" s="17"/>
+      <c r="A133" s="21"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="20"/>
     </row>
     <row r="134">
-      <c r="A134" s="18"/>
-      <c r="B134" s="18"/>
-      <c r="C134" s="17"/>
+      <c r="A134" s="21"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="20"/>
     </row>
     <row r="135">
-      <c r="A135" s="18"/>
-      <c r="B135" s="18"/>
-      <c r="C135" s="17"/>
+      <c r="A135" s="21"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="20"/>
     </row>
     <row r="136">
-      <c r="A136" s="18"/>
-      <c r="B136" s="18"/>
-      <c r="C136" s="17"/>
+      <c r="A136" s="21"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="20"/>
     </row>
     <row r="137">
-      <c r="A137" s="18"/>
-      <c r="B137" s="18"/>
-      <c r="C137" s="17"/>
+      <c r="A137" s="21"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="20"/>
     </row>
     <row r="138">
-      <c r="A138" s="18"/>
-      <c r="B138" s="18"/>
-      <c r="C138" s="17"/>
+      <c r="A138" s="21"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="20"/>
     </row>
     <row r="139">
-      <c r="A139" s="18"/>
-      <c r="B139" s="18"/>
-      <c r="C139" s="17"/>
+      <c r="A139" s="21"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="20"/>
     </row>
     <row r="140">
-      <c r="A140" s="18"/>
-      <c r="B140" s="18"/>
-      <c r="C140" s="17"/>
+      <c r="A140" s="21"/>
+      <c r="B140" s="21"/>
+      <c r="C140" s="20"/>
     </row>
     <row r="141">
-      <c r="A141" s="18"/>
-      <c r="B141" s="18"/>
-      <c r="C141" s="17"/>
+      <c r="A141" s="21"/>
+      <c r="B141" s="21"/>
+      <c r="C141" s="20"/>
     </row>
     <row r="142">
-      <c r="A142" s="18"/>
-      <c r="B142" s="18"/>
-      <c r="C142" s="17"/>
+      <c r="A142" s="21"/>
+      <c r="B142" s="21"/>
+      <c r="C142" s="20"/>
     </row>
     <row r="143">
-      <c r="A143" s="18"/>
-      <c r="B143" s="18"/>
-      <c r="C143" s="17"/>
+      <c r="A143" s="21"/>
+      <c r="B143" s="21"/>
+      <c r="C143" s="20"/>
     </row>
     <row r="144">
-      <c r="A144" s="18"/>
-      <c r="B144" s="18"/>
-      <c r="C144" s="17"/>
+      <c r="A144" s="21"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="20"/>
     </row>
     <row r="145">
-      <c r="A145" s="18"/>
-      <c r="B145" s="18"/>
-      <c r="C145" s="17"/>
+      <c r="A145" s="21"/>
+      <c r="B145" s="21"/>
+      <c r="C145" s="20"/>
     </row>
     <row r="146">
-      <c r="A146" s="18"/>
-      <c r="B146" s="18"/>
-      <c r="C146" s="17"/>
+      <c r="A146" s="21"/>
+      <c r="B146" s="21"/>
+      <c r="C146" s="20"/>
     </row>
     <row r="147">
-      <c r="A147" s="18"/>
-      <c r="B147" s="18"/>
-      <c r="C147" s="17"/>
+      <c r="A147" s="21"/>
+      <c r="B147" s="21"/>
+      <c r="C147" s="20"/>
     </row>
     <row r="148">
-      <c r="A148" s="18"/>
-      <c r="B148" s="18"/>
-      <c r="C148" s="17"/>
+      <c r="A148" s="21"/>
+      <c r="B148" s="21"/>
+      <c r="C148" s="20"/>
     </row>
     <row r="149">
-      <c r="A149" s="18"/>
-      <c r="B149" s="18"/>
-      <c r="C149" s="17"/>
+      <c r="A149" s="21"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="20"/>
     </row>
     <row r="150">
-      <c r="A150" s="18"/>
-      <c r="B150" s="18"/>
-      <c r="C150" s="17"/>
+      <c r="A150" s="21"/>
+      <c r="B150" s="21"/>
+      <c r="C150" s="20"/>
     </row>
     <row r="151">
-      <c r="A151" s="18"/>
-      <c r="B151" s="18"/>
-      <c r="C151" s="17"/>
+      <c r="A151" s="21"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="20"/>
     </row>
     <row r="152">
-      <c r="A152" s="18"/>
-      <c r="B152" s="18"/>
-      <c r="C152" s="17"/>
+      <c r="A152" s="21"/>
+      <c r="B152" s="21"/>
+      <c r="C152" s="20"/>
     </row>
     <row r="153">
-      <c r="A153" s="18"/>
-      <c r="B153" s="18"/>
-      <c r="C153" s="17"/>
+      <c r="A153" s="21"/>
+      <c r="B153" s="21"/>
+      <c r="C153" s="20"/>
     </row>
     <row r="154">
-      <c r="A154" s="18"/>
-      <c r="B154" s="18"/>
-      <c r="C154" s="17"/>
+      <c r="A154" s="21"/>
+      <c r="B154" s="21"/>
+      <c r="C154" s="20"/>
     </row>
     <row r="155">
-      <c r="A155" s="18"/>
-      <c r="B155" s="18"/>
-      <c r="C155" s="17"/>
+      <c r="A155" s="21"/>
+      <c r="B155" s="21"/>
+      <c r="C155" s="20"/>
     </row>
     <row r="156">
-      <c r="A156" s="18"/>
-      <c r="B156" s="18"/>
-      <c r="C156" s="17"/>
+      <c r="A156" s="21"/>
+      <c r="B156" s="21"/>
+      <c r="C156" s="20"/>
     </row>
     <row r="157">
-      <c r="A157" s="18"/>
-      <c r="B157" s="18"/>
-      <c r="C157" s="17"/>
+      <c r="A157" s="21"/>
+      <c r="B157" s="21"/>
+      <c r="C157" s="20"/>
     </row>
     <row r="158">
-      <c r="A158" s="18"/>
-      <c r="B158" s="18"/>
-      <c r="C158" s="17"/>
+      <c r="A158" s="21"/>
+      <c r="B158" s="21"/>
+      <c r="C158" s="20"/>
     </row>
     <row r="159">
-      <c r="A159" s="18"/>
-      <c r="B159" s="18"/>
+      <c r="A159" s="21"/>
+      <c r="B159" s="21"/>
     </row>
     <row r="160">
-      <c r="A160" s="18"/>
-      <c r="B160" s="18"/>
+      <c r="A160" s="21"/>
+      <c r="B160" s="21"/>
     </row>
     <row r="161">
-      <c r="A161" s="18"/>
-      <c r="B161" s="18"/>
+      <c r="A161" s="21"/>
+      <c r="B161" s="21"/>
     </row>
     <row r="162">
-      <c r="A162" s="18"/>
-      <c r="B162" s="18"/>
+      <c r="A162" s="21"/>
+      <c r="B162" s="21"/>
     </row>
     <row r="163">
-      <c r="A163" s="18"/>
-      <c r="B163" s="18"/>
+      <c r="A163" s="21"/>
+      <c r="B163" s="21"/>
     </row>
     <row r="164">
-      <c r="A164" s="18"/>
-      <c r="B164" s="18"/>
+      <c r="A164" s="21"/>
+      <c r="B164" s="21"/>
     </row>
     <row r="165">
-      <c r="A165" s="18"/>
-      <c r="B165" s="18"/>
+      <c r="A165" s="21"/>
+      <c r="B165" s="21"/>
     </row>
     <row r="166">
-      <c r="A166" s="18"/>
-      <c r="B166" s="18"/>
+      <c r="A166" s="21"/>
+      <c r="B166" s="21"/>
     </row>
     <row r="167">
-      <c r="A167" s="18"/>
-      <c r="B167" s="18"/>
+      <c r="A167" s="21"/>
+      <c r="B167" s="21"/>
     </row>
     <row r="168">
-      <c r="A168" s="18"/>
-      <c r="B168" s="18"/>
+      <c r="A168" s="21"/>
+      <c r="B168" s="21"/>
     </row>
     <row r="169">
-      <c r="A169" s="18"/>
-      <c r="B169" s="18"/>
+      <c r="A169" s="21"/>
+      <c r="B169" s="21"/>
     </row>
     <row r="170">
-      <c r="A170" s="18"/>
-      <c r="B170" s="18"/>
+      <c r="A170" s="21"/>
+      <c r="B170" s="21"/>
     </row>
     <row r="171">
-      <c r="A171" s="18"/>
-      <c r="B171" s="18"/>
+      <c r="A171" s="21"/>
+      <c r="B171" s="21"/>
     </row>
     <row r="172">
-      <c r="A172" s="18"/>
-      <c r="B172" s="18"/>
+      <c r="A172" s="21"/>
+      <c r="B172" s="21"/>
     </row>
     <row r="173">
-      <c r="A173" s="18"/>
-      <c r="B173" s="18"/>
+      <c r="A173" s="21"/>
+      <c r="B173" s="21"/>
     </row>
     <row r="174">
-      <c r="A174" s="18"/>
-      <c r="B174" s="18"/>
+      <c r="A174" s="21"/>
+      <c r="B174" s="21"/>
     </row>
     <row r="175">
-      <c r="A175" s="18"/>
-      <c r="B175" s="18"/>
+      <c r="A175" s="21"/>
+      <c r="B175" s="21"/>
     </row>
     <row r="176">
-      <c r="A176" s="18"/>
-      <c r="B176" s="18"/>
+      <c r="A176" s="21"/>
+      <c r="B176" s="21"/>
     </row>
     <row r="177">
-      <c r="A177" s="18"/>
-      <c r="B177" s="18"/>
+      <c r="A177" s="21"/>
+      <c r="B177" s="21"/>
     </row>
     <row r="178">
-      <c r="A178" s="18"/>
-      <c r="B178" s="18"/>
+      <c r="A178" s="21"/>
+      <c r="B178" s="21"/>
     </row>
     <row r="179">
-      <c r="A179" s="18"/>
-      <c r="B179" s="18"/>
+      <c r="A179" s="21"/>
+      <c r="B179" s="21"/>
     </row>
     <row r="180">
-      <c r="A180" s="18"/>
-      <c r="B180" s="18"/>
+      <c r="A180" s="21"/>
+      <c r="B180" s="21"/>
     </row>
     <row r="181">
-      <c r="A181" s="18"/>
-      <c r="B181" s="18"/>
+      <c r="A181" s="21"/>
+      <c r="B181" s="21"/>
     </row>
     <row r="182">
-      <c r="A182" s="18"/>
-      <c r="B182" s="18"/>
+      <c r="A182" s="21"/>
+      <c r="B182" s="21"/>
     </row>
     <row r="183">
-      <c r="A183" s="18"/>
-      <c r="B183" s="18"/>
+      <c r="A183" s="21"/>
+      <c r="B183" s="21"/>
     </row>
     <row r="184">
-      <c r="A184" s="18"/>
-      <c r="B184" s="18"/>
+      <c r="A184" s="21"/>
+      <c r="B184" s="21"/>
     </row>
     <row r="185">
-      <c r="A185" s="18"/>
-      <c r="B185" s="18"/>
+      <c r="A185" s="21"/>
+      <c r="B185" s="21"/>
     </row>
     <row r="186">
-      <c r="A186" s="18"/>
-      <c r="B186" s="18"/>
+      <c r="A186" s="21"/>
+      <c r="B186" s="21"/>
     </row>
     <row r="187">
-      <c r="A187" s="18"/>
-      <c r="B187" s="18"/>
+      <c r="A187" s="21"/>
+      <c r="B187" s="21"/>
     </row>
     <row r="188">
-      <c r="A188" s="18"/>
-      <c r="B188" s="18"/>
+      <c r="A188" s="21"/>
+      <c r="B188" s="21"/>
     </row>
     <row r="189">
-      <c r="A189" s="18"/>
-      <c r="B189" s="18"/>
+      <c r="A189" s="21"/>
+      <c r="B189" s="21"/>
     </row>
     <row r="190">
-      <c r="A190" s="18"/>
-      <c r="B190" s="18"/>
+      <c r="A190" s="21"/>
+      <c r="B190" s="21"/>
     </row>
     <row r="191">
-      <c r="A191" s="18"/>
-      <c r="B191" s="18"/>
+      <c r="A191" s="21"/>
+      <c r="B191" s="21"/>
     </row>
     <row r="192">
-      <c r="A192" s="18"/>
-      <c r="B192" s="18"/>
+      <c r="A192" s="21"/>
+      <c r="B192" s="21"/>
     </row>
     <row r="193">
-      <c r="A193" s="18"/>
-      <c r="B193" s="18"/>
+      <c r="A193" s="21"/>
+      <c r="B193" s="21"/>
     </row>
     <row r="194">
-      <c r="A194" s="18"/>
-      <c r="B194" s="18"/>
+      <c r="A194" s="21"/>
+      <c r="B194" s="21"/>
     </row>
     <row r="195">
-      <c r="A195" s="18"/>
-      <c r="B195" s="18"/>
+      <c r="A195" s="21"/>
+      <c r="B195" s="21"/>
     </row>
     <row r="196">
-      <c r="A196" s="18"/>
-      <c r="B196" s="18"/>
+      <c r="A196" s="21"/>
+      <c r="B196" s="21"/>
     </row>
     <row r="197">
-      <c r="A197" s="18"/>
-      <c r="B197" s="18"/>
+      <c r="A197" s="21"/>
+      <c r="B197" s="21"/>
     </row>
     <row r="198">
-      <c r="A198" s="18"/>
-      <c r="B198" s="18"/>
+      <c r="A198" s="21"/>
+      <c r="B198" s="21"/>
     </row>
     <row r="199">
-      <c r="A199" s="18"/>
-      <c r="B199" s="18"/>
+      <c r="A199" s="21"/>
+      <c r="B199" s="21"/>
     </row>
     <row r="200">
-      <c r="A200" s="18"/>
-      <c r="B200" s="18"/>
+      <c r="A200" s="21"/>
+      <c r="B200" s="21"/>
     </row>
     <row r="201">
-      <c r="A201" s="18"/>
-      <c r="B201" s="18"/>
+      <c r="A201" s="21"/>
+      <c r="B201" s="21"/>
     </row>
     <row r="202">
-      <c r="A202" s="18"/>
-      <c r="B202" s="18"/>
+      <c r="A202" s="21"/>
+      <c r="B202" s="21"/>
     </row>
     <row r="203">
-      <c r="A203" s="18"/>
-      <c r="B203" s="18"/>
+      <c r="A203" s="21"/>
+      <c r="B203" s="21"/>
     </row>
     <row r="204">
-      <c r="A204" s="18"/>
-      <c r="B204" s="18"/>
+      <c r="A204" s="21"/>
+      <c r="B204" s="21"/>
     </row>
     <row r="205">
-      <c r="A205" s="18"/>
-      <c r="B205" s="18"/>
+      <c r="A205" s="21"/>
+      <c r="B205" s="21"/>
     </row>
     <row r="206">
-      <c r="A206" s="18"/>
-      <c r="B206" s="18"/>
+      <c r="A206" s="21"/>
+      <c r="B206" s="21"/>
     </row>
     <row r="207">
-      <c r="A207" s="18"/>
-      <c r="B207" s="18"/>
+      <c r="A207" s="21"/>
+      <c r="B207" s="21"/>
     </row>
     <row r="208">
-      <c r="A208" s="18"/>
-      <c r="B208" s="18"/>
+      <c r="A208" s="21"/>
+      <c r="B208" s="21"/>
     </row>
     <row r="209">
-      <c r="A209" s="18"/>
-      <c r="B209" s="18"/>
+      <c r="A209" s="21"/>
+      <c r="B209" s="21"/>
     </row>
     <row r="210">
-      <c r="A210" s="18"/>
-      <c r="B210" s="18"/>
+      <c r="A210" s="21"/>
+      <c r="B210" s="21"/>
     </row>
     <row r="211">
-      <c r="A211" s="18"/>
-      <c r="B211" s="18"/>
+      <c r="A211" s="21"/>
+      <c r="B211" s="21"/>
     </row>
     <row r="212">
-      <c r="A212" s="18"/>
-      <c r="B212" s="18"/>
+      <c r="A212" s="21"/>
+      <c r="B212" s="21"/>
     </row>
     <row r="213">
-      <c r="A213" s="18"/>
-      <c r="B213" s="18"/>
+      <c r="A213" s="21"/>
+      <c r="B213" s="21"/>
     </row>
     <row r="214">
-      <c r="A214" s="18"/>
-      <c r="B214" s="18"/>
+      <c r="A214" s="21"/>
+      <c r="B214" s="21"/>
     </row>
     <row r="215">
-      <c r="A215" s="18"/>
-      <c r="B215" s="18"/>
+      <c r="A215" s="21"/>
+      <c r="B215" s="21"/>
     </row>
     <row r="216">
-      <c r="A216" s="18"/>
-      <c r="B216" s="18"/>
+      <c r="A216" s="21"/>
+      <c r="B216" s="21"/>
     </row>
     <row r="217">
-      <c r="A217" s="18"/>
-      <c r="B217" s="18"/>
+      <c r="A217" s="21"/>
+      <c r="B217" s="21"/>
     </row>
     <row r="218">
-      <c r="A218" s="18"/>
-      <c r="B218" s="18"/>
+      <c r="A218" s="21"/>
+      <c r="B218" s="21"/>
     </row>
     <row r="219">
-      <c r="A219" s="18"/>
-      <c r="B219" s="18"/>
+      <c r="A219" s="21"/>
+      <c r="B219" s="21"/>
     </row>
     <row r="220">
-      <c r="A220" s="18"/>
-      <c r="B220" s="18"/>
+      <c r="A220" s="21"/>
+      <c r="B220" s="21"/>
     </row>
     <row r="221">
-      <c r="A221" s="18"/>
-      <c r="B221" s="18"/>
+      <c r="A221" s="21"/>
+      <c r="B221" s="21"/>
     </row>
     <row r="222">
-      <c r="A222" s="18"/>
-      <c r="B222" s="18"/>
+      <c r="A222" s="21"/>
+      <c r="B222" s="21"/>
     </row>
     <row r="223">
-      <c r="A223" s="18"/>
-      <c r="B223" s="18"/>
+      <c r="A223" s="21"/>
+      <c r="B223" s="21"/>
     </row>
     <row r="224">
-      <c r="A224" s="18"/>
-      <c r="B224" s="18"/>
+      <c r="A224" s="21"/>
+      <c r="B224" s="21"/>
     </row>
     <row r="225">
-      <c r="A225" s="18"/>
-      <c r="B225" s="18"/>
+      <c r="A225" s="21"/>
+      <c r="B225" s="21"/>
     </row>
     <row r="226">
-      <c r="A226" s="18"/>
-      <c r="B226" s="18"/>
+      <c r="A226" s="21"/>
+      <c r="B226" s="21"/>
     </row>
     <row r="227">
-      <c r="A227" s="18"/>
-      <c r="B227" s="18"/>
+      <c r="A227" s="21"/>
+      <c r="B227" s="21"/>
     </row>
     <row r="228">
-      <c r="A228" s="18"/>
-      <c r="B228" s="18"/>
+      <c r="A228" s="21"/>
+      <c r="B228" s="21"/>
     </row>
     <row r="229">
-      <c r="A229" s="18"/>
-      <c r="B229" s="18"/>
+      <c r="A229" s="21"/>
+      <c r="B229" s="21"/>
     </row>
     <row r="230">
-      <c r="A230" s="18"/>
-      <c r="B230" s="18"/>
+      <c r="A230" s="21"/>
+      <c r="B230" s="21"/>
     </row>
     <row r="231">
-      <c r="A231" s="18"/>
-      <c r="B231" s="18"/>
+      <c r="A231" s="21"/>
+      <c r="B231" s="21"/>
     </row>
     <row r="232">
-      <c r="A232" s="18"/>
-      <c r="B232" s="18"/>
+      <c r="A232" s="21"/>
+      <c r="B232" s="21"/>
     </row>
     <row r="233">
-      <c r="A233" s="18"/>
-      <c r="B233" s="18"/>
+      <c r="A233" s="21"/>
+      <c r="B233" s="21"/>
     </row>
     <row r="234">
-      <c r="A234" s="18"/>
-      <c r="B234" s="18"/>
+      <c r="A234" s="21"/>
+      <c r="B234" s="21"/>
     </row>
     <row r="235">
-      <c r="A235" s="18"/>
-      <c r="B235" s="18"/>
+      <c r="A235" s="21"/>
+      <c r="B235" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -6531,12 +6579,12 @@
   <sheetData>
     <row r="1" ht="30.449999999999999" customHeight="1">
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -6545,7 +6593,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -6555,20 +6603,20 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
@@ -6576,135 +6624,135 @@
       <c r="AJ1" s="1"/>
     </row>
     <row r="2" ht="106.2" customHeight="1">
-      <c r="B2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="B2" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="22" t="s">
+      <c r="H2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="22" t="s">
+      <c r="J2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="K2" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="22" t="s">
+      <c r="L2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="M2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="N2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="22" t="s">
+      <c r="O2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="22" t="s">
+      <c r="P2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="23" t="s">
+      <c r="Q2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="S2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="22" t="s">
+      <c r="T2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="22" t="s">
+      <c r="U2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="V2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="W2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="X2" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="Y2" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AE2" s="26" t="s">
+      <c r="Z2" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AF2" s="26" t="s">
+      <c r="AA2" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="AG2" s="26" t="s">
+      <c r="AB2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AC2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="AI2" s="26" t="s">
+      <c r="AD2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="AJ2" s="26" t="s">
+      <c r="AE2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="27"/>
-      <c r="AR2" s="27"/>
-      <c r="AS2" s="27"/>
-      <c r="AT2" s="27"/>
-      <c r="AU2" s="27"/>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27"/>
+      <c r="AF2" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
+      <c r="AN2" s="30"/>
+      <c r="AO2" s="30"/>
+      <c r="AP2" s="30"/>
+      <c r="AQ2" s="30"/>
+      <c r="AR2" s="30"/>
+      <c r="AS2" s="30"/>
+      <c r="AT2" s="30"/>
+      <c r="AU2" s="30"/>
+      <c r="AV2" s="30"/>
+      <c r="AW2" s="30"/>
     </row>
     <row r="55">
-      <c r="D55" s="28"/>
+      <c r="D55" s="31"/>
     </row>
     <row r="56">
-      <c r="C56" s="29"/>
-      <c r="D56" s="30"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
     </row>
     <row r="57">
-      <c r="C57" s="29"/>
-      <c r="D57" s="31"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -6748,801 +6796,801 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="32"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" ht="56.399999999999999" customHeight="1">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="38"/>
-      <c r="AD2" s="39"/>
+      <c r="S2" s="41"/>
+      <c r="AD2" s="42"/>
     </row>
     <row r="3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="43">
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="46">
         <v>4</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F3" s="47">
         <v>1</v>
       </c>
-      <c r="G3" s="45">
+      <c r="G3" s="48">
         <v>2</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="48">
         <v>3</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="46">
         <v>4</v>
       </c>
-      <c r="J3" s="44">
+      <c r="J3" s="47">
         <v>1</v>
       </c>
-      <c r="K3" s="45">
+      <c r="K3" s="48">
         <v>2</v>
       </c>
-      <c r="L3" s="45">
+      <c r="L3" s="48">
         <v>3</v>
       </c>
-      <c r="M3" s="43">
+      <c r="M3" s="46">
         <v>4</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="47">
         <v>1</v>
       </c>
-      <c r="O3" s="45">
+      <c r="O3" s="48">
         <v>2</v>
       </c>
-      <c r="P3" s="45">
+      <c r="P3" s="48">
         <v>3</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="46">
         <v>4</v>
       </c>
-      <c r="R3" s="44">
+      <c r="R3" s="47">
         <v>1</v>
       </c>
-      <c r="S3" s="46">
+      <c r="S3" s="49">
         <v>2</v>
       </c>
       <c r="U3" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" ht="12" customHeight="1">
-      <c r="B4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="53"/>
+      <c r="B4" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="56"/>
       <c r="U4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" ht="12" customHeight="1">
-      <c r="B5" s="47"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="61"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="64"/>
     </row>
     <row r="6" ht="12" customHeight="1">
-      <c r="B6" s="47"/>
-      <c r="C6" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="69"/>
-      <c r="U6" s="70" t="s">
-        <v>76</v>
-      </c>
-      <c r="V6" s="70"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="72"/>
+      <c r="U6" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="V6" s="73"/>
     </row>
     <row r="7" ht="12" customHeight="1">
-      <c r="B7" s="47"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="61"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="64"/>
       <c r="U7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1">
-      <c r="B8" s="47"/>
-      <c r="C8" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="69"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="72"/>
       <c r="U8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" ht="12" customHeight="1">
-      <c r="B9" s="47"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="61"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="64"/>
     </row>
     <row r="10" ht="12" customHeight="1">
-      <c r="B10" s="47"/>
-      <c r="C10" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="69"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="72"/>
     </row>
     <row r="11" ht="12" customHeight="1">
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="78"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="78"/>
+      <c r="S11" s="81"/>
     </row>
     <row r="12" ht="12" customHeight="1">
-      <c r="B12" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="49"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="53"/>
+      <c r="B12" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="56"/>
     </row>
     <row r="13" ht="12" customHeight="1">
-      <c r="B13" s="47"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="61"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="64"/>
     </row>
     <row r="14" ht="12" customHeight="1">
-      <c r="B14" s="47"/>
-      <c r="C14" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="64"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="67"/>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="84"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="72"/>
     </row>
     <row r="15" ht="12" customHeight="1">
-      <c r="B15" s="47"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="82"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="61"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="64"/>
     </row>
     <row r="16" ht="12" customHeight="1">
-      <c r="B16" s="47"/>
-      <c r="C16" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="64"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="67"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="68"/>
-      <c r="S16" s="69"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="72"/>
     </row>
     <row r="17" ht="12" customHeight="1">
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="78"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="77"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="81"/>
     </row>
     <row r="18" ht="12" customHeight="1">
-      <c r="B18" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="52"/>
-      <c r="S18" s="53"/>
+      <c r="B18" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="56"/>
     </row>
     <row r="19" ht="12" customHeight="1">
-      <c r="B19" s="47"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="61"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="64"/>
     </row>
     <row r="20" ht="12" customHeight="1">
-      <c r="B20" s="47"/>
-      <c r="C20" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="63"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="67"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="68"/>
-      <c r="S20" s="69"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="70"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="72"/>
     </row>
     <row r="21" ht="12" customHeight="1">
-      <c r="B21" s="47"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="61"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="64"/>
     </row>
     <row r="22" ht="12" customHeight="1">
-      <c r="B22" s="47"/>
-      <c r="C22" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="63"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="64"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="64"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="69"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="72"/>
     </row>
     <row r="23" ht="12" customHeight="1">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="75"/>
-      <c r="S23" s="78"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="77"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="81"/>
     </row>
     <row r="24" ht="12" customHeight="1">
-      <c r="B24" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="80"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="53"/>
+      <c r="B24" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="82"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
     <row r="25" ht="12" customHeight="1">
-      <c r="B25" s="47"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="61"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="64"/>
     </row>
     <row r="26" ht="12" customHeight="1">
-      <c r="B26" s="47"/>
-      <c r="C26" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="66"/>
-      <c r="P26" s="66"/>
-      <c r="Q26" s="64"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="69"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="72"/>
     </row>
     <row r="27" ht="12" customHeight="1">
-      <c r="B27" s="47"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="56"/>
-      <c r="R27" s="60"/>
-      <c r="S27" s="61"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="64"/>
     </row>
     <row r="28" ht="12" customHeight="1">
-      <c r="B28" s="47"/>
-      <c r="C28" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="68"/>
-      <c r="O28" s="67"/>
-      <c r="P28" s="66"/>
-      <c r="Q28" s="83"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="69"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="86"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="72"/>
     </row>
     <row r="29" ht="12" customHeight="1">
-      <c r="B29" s="47"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="88"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="91"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="89"/>
-      <c r="Q29" s="87"/>
-      <c r="R29" s="88"/>
-      <c r="S29" s="92"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="93"/>
+      <c r="P29" s="92"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="91"/>
+      <c r="S29" s="95"/>
     </row>
     <row r="30" ht="12" customHeight="1">
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="94" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="48"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="97"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="96"/>
-      <c r="K30" s="96"/>
-      <c r="L30" s="97"/>
-      <c r="M30" s="98"/>
-      <c r="N30" s="96"/>
-      <c r="O30" s="97"/>
-      <c r="P30" s="96"/>
-      <c r="Q30" s="98"/>
-      <c r="R30" s="96"/>
-      <c r="S30" s="99"/>
+      <c r="C30" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="51"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="99"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="99"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="102"/>
     </row>
     <row r="31" ht="12" customHeight="1">
-      <c r="B31" s="100"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="102"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="104"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="104"/>
-      <c r="M31" s="105"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="104"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="105"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="61"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="64"/>
     </row>
     <row r="32" ht="12" customHeight="1">
-      <c r="B32" s="100"/>
-      <c r="C32" s="101" t="s">
+      <c r="B32" s="103"/>
+      <c r="C32" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="107"/>
-      <c r="F32" s="108"/>
-      <c r="G32" s="108"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="108"/>
-      <c r="K32" s="108"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="110"/>
-      <c r="N32" s="108"/>
-      <c r="O32" s="109"/>
-      <c r="P32" s="108"/>
-      <c r="Q32" s="110"/>
-      <c r="R32" s="108"/>
-      <c r="S32" s="111"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="112"/>
+      <c r="M32" s="113"/>
+      <c r="N32" s="111"/>
+      <c r="O32" s="112"/>
+      <c r="P32" s="111"/>
+      <c r="Q32" s="113"/>
+      <c r="R32" s="111"/>
+      <c r="S32" s="114"/>
     </row>
     <row r="33" ht="12" customHeight="1">
-      <c r="B33" s="100"/>
-      <c r="C33" s="101"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="106"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="112"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="103"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="105"/>
-      <c r="N33" s="103"/>
-      <c r="O33" s="104"/>
-      <c r="P33" s="103"/>
-      <c r="Q33" s="105"/>
-      <c r="R33" s="103"/>
-      <c r="S33" s="61"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="115"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="107"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="64"/>
     </row>
     <row r="34" ht="12" customHeight="1">
-      <c r="B34" s="100"/>
-      <c r="C34" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="114"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="117"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="115"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="117"/>
-      <c r="N34" s="115"/>
-      <c r="O34" s="116"/>
-      <c r="P34" s="115"/>
-      <c r="Q34" s="117"/>
-      <c r="R34" s="115"/>
-      <c r="S34" s="118"/>
-      <c r="U34" s="119"/>
-      <c r="V34" s="120" t="s">
-        <v>95</v>
+      <c r="B34" s="103"/>
+      <c r="C34" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="89"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="118"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="120"/>
+      <c r="N34" s="118"/>
+      <c r="O34" s="119"/>
+      <c r="P34" s="118"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="118"/>
+      <c r="S34" s="121"/>
+      <c r="U34" s="122"/>
+      <c r="V34" s="123" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" ht="13.800000000000001" customHeight="1">
-      <c r="B35" s="121"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="123"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="124"/>
-      <c r="H35" s="125"/>
-      <c r="I35" s="126"/>
-      <c r="J35" s="124"/>
-      <c r="K35" s="124"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="126"/>
-      <c r="N35" s="124"/>
-      <c r="O35" s="125"/>
-      <c r="P35" s="124"/>
-      <c r="Q35" s="126"/>
-      <c r="R35" s="124"/>
-      <c r="S35" s="78"/>
-      <c r="U35" s="31"/>
-      <c r="V35" s="127" t="s">
-        <v>96</v>
+      <c r="B35" s="124"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="127"/>
+      <c r="G35" s="127"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="127"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="129"/>
+      <c r="N35" s="127"/>
+      <c r="O35" s="128"/>
+      <c r="P35" s="127"/>
+      <c r="Q35" s="129"/>
+      <c r="R35" s="127"/>
+      <c r="S35" s="81"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="130" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commencement du diagramme de classe des données
Classe de connexion à la BDD
</commit_message>
<xml_diff>
--- a/Documentation/HoferL-JournalPlanif-M5.xlsx
+++ b/Documentation/HoferL-JournalPlanif-M5.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>date</t>
   </si>
@@ -120,10 +120,16 @@
     <t xml:space="preserve">Création de diagrammes (cas utilisation, MCD, classe), mis en pause, analyse pas terminé.</t>
   </si>
   <si>
-    <t>05.02.2026</t>
+    <t>06.02-2026</t>
   </si>
   <si>
     <t xml:space="preserve">Finalisation de la documentation analyse de l'application. </t>
+  </si>
+  <si>
+    <t>06.02.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commencement du chapitre conception de l'applicaiton. MCD et Diagramme de Classes. Relecture du document.</t>
   </si>
   <si>
     <t>Janvier</t>
@@ -1207,14 +1213,14 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="167" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3743,8 +3749,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Journal" ref="B2:E16">
-  <autoFilter ref="B2:E16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Journal" ref="B2:E17">
+  <autoFilter ref="B2:E17"/>
   <tableColumns count="4">
     <tableColumn id="1" name="date" dataDxfId="0"/>
     <tableColumn id="2" name="Temps" dataDxfId="1"/>
@@ -4256,7 +4262,7 @@
       <selection activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="2"/>
     <col customWidth="1" min="2" max="2" width="11.33203125"/>
@@ -4339,7 +4345,7 @@
         <v>0.045454545454545456</v>
       </c>
     </row>
-    <row r="5" ht="28.800000000000001">
+    <row r="5" ht="28.5">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="8" ht="28.800000000000001">
+    <row r="8" ht="28.5">
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" ht="29.399999999999999">
+    <row r="11" ht="28.5">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -4525,7 +4531,7 @@
       </c>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" ht="43.200000000000003">
+    <row r="13" ht="42.75">
       <c r="B13" s="3">
         <v>46056</v>
       </c>
@@ -4540,53 +4546,61 @@
       </c>
       <c r="H13" s="8"/>
     </row>
-    <row r="14">
+    <row r="14" ht="28.5">
       <c r="B14" s="13">
         <v>46057</v>
       </c>
       <c r="C14" s="4">
         <v>0.083333333333333329</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="16" t="s">
+    <row r="15" ht="28.5">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="4">
         <v>0.125</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="4">
         <v>0.125</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
+    <row r="17" ht="28.5">
+      <c r="B17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" s="3"/>
@@ -4970,7 +4984,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="1">
-        <x14:dataValidation xr:uid="{000A003D-0045-4696-AF39-006300EB0054}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{009B00F6-0014-40AF-A56B-004100B90060}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$G$3:$G$7</xm:f>
           </x14:formula1>
@@ -6579,12 +6593,12 @@
   <sheetData>
     <row r="1" ht="30.449999999999999" customHeight="1">
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -6593,7 +6607,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -6603,20 +6617,20 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
@@ -6625,109 +6639,109 @@
     </row>
     <row r="2" ht="106.2" customHeight="1">
       <c r="B2" s="22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G2" s="25" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I2" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M2" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="25" t="s">
-        <v>46</v>
-      </c>
       <c r="R2" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S2" s="25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T2" s="25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U2" s="25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="W2" s="26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="X2" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB2" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC2" s="27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AD2" s="28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AE2" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF2" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AG2" s="29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AH2" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AI2" s="29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AJ2" s="29" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AK2" s="30"/>
       <c r="AL2" s="30"/>
@@ -6800,37 +6814,37 @@
     </row>
     <row r="2" ht="56.399999999999999" customHeight="1">
       <c r="B2" s="36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="40"/>
       <c r="I2" s="39"/>
       <c r="J2" s="40" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K2" s="40"/>
       <c r="L2" s="40"/>
       <c r="M2" s="39"/>
       <c r="N2" s="40" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O2" s="40"/>
       <c r="P2" s="40"/>
       <c r="Q2" s="39"/>
       <c r="R2" s="40" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S2" s="41"/>
       <c r="AD2" s="42"/>
@@ -6839,7 +6853,7 @@
       <c r="B3" s="43"/>
       <c r="C3" s="44"/>
       <c r="D3" s="45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E3" s="46">
         <v>4</v>
@@ -6887,15 +6901,15 @@
         <v>2</v>
       </c>
       <c r="U3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" ht="12" customHeight="1">
       <c r="B4" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="52"/>
@@ -6914,7 +6928,7 @@
       <c r="R4" s="55"/>
       <c r="S4" s="56"/>
       <c r="U4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" ht="12" customHeight="1">
@@ -6940,7 +6954,7 @@
     <row r="6" ht="12" customHeight="1">
       <c r="B6" s="50"/>
       <c r="C6" s="65" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D6" s="66"/>
       <c r="E6" s="67"/>
@@ -6959,7 +6973,7 @@
       <c r="R6" s="71"/>
       <c r="S6" s="72"/>
       <c r="U6" s="73" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="V6" s="73"/>
     </row>
@@ -6983,13 +6997,13 @@
       <c r="R7" s="63"/>
       <c r="S7" s="64"/>
       <c r="U7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1">
       <c r="B8" s="50"/>
       <c r="C8" s="65" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D8" s="66"/>
       <c r="E8" s="67"/>
@@ -7008,7 +7022,7 @@
       <c r="R8" s="71"/>
       <c r="S8" s="72"/>
       <c r="U8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" ht="12" customHeight="1">
@@ -7034,7 +7048,7 @@
     <row r="10" ht="12" customHeight="1">
       <c r="B10" s="50"/>
       <c r="C10" s="65" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D10" s="66"/>
       <c r="E10" s="67"/>
@@ -7075,10 +7089,10 @@
     </row>
     <row r="12" ht="12" customHeight="1">
       <c r="B12" s="36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D12" s="51"/>
       <c r="E12" s="52"/>
@@ -7120,7 +7134,7 @@
     <row r="14" ht="12" customHeight="1">
       <c r="B14" s="50"/>
       <c r="C14" s="65" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="67"/>
@@ -7162,7 +7176,7 @@
     <row r="16" ht="12" customHeight="1">
       <c r="B16" s="50"/>
       <c r="C16" s="65" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D16" s="66"/>
       <c r="E16" s="67"/>
@@ -7203,10 +7217,10 @@
     </row>
     <row r="18" ht="12" customHeight="1">
       <c r="B18" s="38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="52"/>
@@ -7248,7 +7262,7 @@
     <row r="20" ht="12" customHeight="1">
       <c r="B20" s="50"/>
       <c r="C20" s="65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D20" s="66"/>
       <c r="E20" s="67"/>
@@ -7290,7 +7304,7 @@
     <row r="22" ht="12" customHeight="1">
       <c r="B22" s="50"/>
       <c r="C22" s="65" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D22" s="66"/>
       <c r="E22" s="67"/>
@@ -7331,10 +7345,10 @@
     </row>
     <row r="24" ht="12" customHeight="1">
       <c r="B24" s="38" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="52"/>
@@ -7376,7 +7390,7 @@
     <row r="26" ht="12" customHeight="1">
       <c r="B26" s="50"/>
       <c r="C26" s="65" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D26" s="66"/>
       <c r="E26" s="67"/>
@@ -7418,7 +7432,7 @@
     <row r="28" ht="12" customHeight="1">
       <c r="B28" s="50"/>
       <c r="C28" s="65" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D28" s="66"/>
       <c r="E28" s="67"/>
@@ -7462,7 +7476,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="97" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D30" s="51"/>
       <c r="E30" s="98"/>
@@ -7546,7 +7560,7 @@
     <row r="34" ht="12" customHeight="1">
       <c r="B34" s="103"/>
       <c r="C34" s="57" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D34" s="89"/>
       <c r="E34" s="117"/>
@@ -7566,7 +7580,7 @@
       <c r="S34" s="121"/>
       <c r="U34" s="122"/>
       <c r="V34" s="123" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" ht="13.800000000000001" customHeight="1">
@@ -7590,7 +7604,7 @@
       <c r="S35" s="81"/>
       <c r="U35" s="34"/>
       <c r="V35" s="130" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalisation du menu journal
Ajout de la maquette dans MD
</commit_message>
<xml_diff>
--- a/Documentation/HoferL-JournalPlanif-M5.xlsx
+++ b/Documentation/HoferL-JournalPlanif-M5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\ScholarLog\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66C9A0A-0D73-4A12-B9A3-0DC611325CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D77F723-3160-4E4E-81C2-6407801350C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
   <si>
     <t>date</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>Finalisation menu Note</t>
+  </si>
+  <si>
+    <t>Finalisation du menu Journal</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,6 +597,12 @@
         <bgColor theme="0" tint="-4.9989318521683403E-2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="69">
     <border>
@@ -1414,7 +1423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1641,11 +1650,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -1657,12 +1668,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1674,8 +1691,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
@@ -1695,35 +1730,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1731,22 +1741,22 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="1" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="hh:mm;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="166" formatCode="0.0&quot; H&quot;;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0&quot; H&quot;;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" relativeIndent="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2113,22 +2123,22 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.8181818181818177E-2</c:v>
+                  <c:v>6.5217391304347824E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8181818181818177E-2</c:v>
+                  <c:v>6.5217391304347824E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13636363636363635</c:v>
+                  <c:v>0.13043478260869565</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20454545454545456</c:v>
+                  <c:v>0.2391304347826087</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47727272727272718</c:v>
+                  <c:v>0.4565217391304347</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5454545454545456E-2</c:v>
+                  <c:v>4.3478260869565216E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2366,7 +2376,7 @@
             <c:strRef>
               <c:f>SommeParJours!$A$2:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>20.01.2026</c:v>
                 </c:pt>
@@ -2393,6 +2403,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.02.2026</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.02.2026</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2429,6 +2442,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.29166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3497,13 +3513,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Journal" displayName="Journal" ref="B2:E22">
-  <autoFilter ref="B2:E22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Journal" displayName="Journal" ref="B2:E23">
+  <autoFilter ref="B2:E23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Temps" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="type de travail" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Temps" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="type de travail" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="description" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3514,7 +3530,7 @@
   <autoFilter ref="G2:H11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="type de travail"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="somme" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="somme" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3723,8 +3739,8 @@
   </sheetPr>
   <dimension ref="B2:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3781,7 +3797,7 @@
       </c>
       <c r="I3" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>6.8181818181818177E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
       <c r="J3" s="10"/>
     </row>
@@ -3807,7 +3823,7 @@
       </c>
       <c r="I4" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>6.8181818181818177E-2</v>
+        <v>6.5217391304347824E-2</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3832,7 +3848,7 @@
       </c>
       <c r="I5" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>0.13636363636363635</v>
+        <v>0.13043478260869565</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -3853,11 +3869,11 @@
       </c>
       <c r="H6" s="8">
         <f>SUMIF(Journal[type de travail],types[[#This Row],[type de travail]],Journal[Temps])*24</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I6" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>0.20454545454545456</v>
+        <v>0.2391304347826087</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -3882,7 +3898,7 @@
       </c>
       <c r="I7" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>0.47727272727272718</v>
+        <v>0.4565217391304347</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3907,7 +3923,7 @@
       </c>
       <c r="I8" s="9">
         <f>types[[#This Row],[somme]]/$H$11</f>
-        <v>4.5454545454545456E-2</v>
+        <v>4.3478260869565216E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -3978,7 +3994,7 @@
       </c>
       <c r="H11" s="8">
         <f>SUM(H3:H10)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -4096,7 +4112,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="164" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="4">
@@ -4110,7 +4126,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="164" t="s">
+      <c r="B21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C21" s="4">
@@ -4124,7 +4140,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="164" t="s">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="4">
@@ -4138,10 +4154,18 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="3">
+        <v>46065</v>
+      </c>
+      <c r="C23" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
@@ -4276,163 +4300,163 @@
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="5"/>
+      <c r="B46" s="164"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="5"/>
+      <c r="B47" s="164"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="5"/>
+      <c r="B48" s="164"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="5"/>
+      <c r="B49" s="164"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="5"/>
+      <c r="B50" s="164"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="5"/>
+      <c r="B51" s="164"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="5"/>
+      <c r="B52" s="164"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="5"/>
+      <c r="B53" s="164"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="5"/>
+      <c r="B54" s="164"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="5"/>
+      <c r="B55" s="164"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="5"/>
+      <c r="B56" s="164"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="5"/>
+      <c r="B57" s="164"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="5"/>
+      <c r="B58" s="164"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="5"/>
+      <c r="B59" s="164"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="5"/>
+      <c r="B60" s="164"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="5"/>
+      <c r="B61" s="164"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="5"/>
+      <c r="B62" s="164"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="5"/>
+      <c r="B63" s="164"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="5"/>
+      <c r="B64" s="164"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="5"/>
+      <c r="B65" s="164"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="5"/>
+      <c r="B66" s="164"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="5"/>
+      <c r="B67" s="164"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="5"/>
+      <c r="B68" s="164"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B69" s="5"/>
+      <c r="B69" s="164"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B70" s="5"/>
+      <c r="B70" s="164"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B71" s="5"/>
+      <c r="B71" s="164"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B72" s="5"/>
+      <c r="B72" s="164"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -4480,15 +4504,15 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LÉcole Supérieur Technique&amp;CJournal de travail - M5&amp;RTINF2</oddHeader>
     <oddFooter>&amp;LHoferL-JournalPlanif-M5.xlsx&amp;RLHO/04.02.2026</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4498,7 +4522,7 @@
   <dimension ref="A1:C235"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4520,7 +4544,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="str" cm="1">
-        <f t="array" ref="A2:A10">_xlfn.UNIQUE(Journal[date])</f>
+        <f t="array" ref="A2:A11">_xlfn.UNIQUE(Journal[date])</f>
         <v>20.01.2026</v>
       </c>
       <c r="B2" s="15">
@@ -4610,8 +4634,13 @@
       <c r="C10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="14">
+        <v>46065</v>
+      </c>
+      <c r="B11" s="15">
+        <f>SUMIF(Journal[date],SommeParJours!A11,Journal[Temps])</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="C11"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -6135,7 +6164,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AD2" sqref="AD2"/>
-      <selection pane="bottomLeft" activeCell="AS25" sqref="AS25"/>
+      <selection pane="bottomLeft" activeCell="AQ32" sqref="AQ32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6274,10 +6303,10 @@
       <c r="AU1" s="34"/>
     </row>
     <row r="2" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="141" t="s">
+      <c r="C2" s="139" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="35"/>
@@ -6316,8 +6345,8 @@
       <c r="AK2" s="35"/>
     </row>
     <row r="3" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="136"/>
-      <c r="C3" s="141"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
       <c r="F3" s="43"/>
@@ -6354,8 +6383,8 @@
       <c r="AK3" s="35"/>
     </row>
     <row r="4" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="136"/>
-      <c r="C4" s="141" t="s">
+      <c r="B4" s="138"/>
+      <c r="C4" s="139" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="35"/>
@@ -6394,8 +6423,8 @@
       <c r="AK4" s="35"/>
     </row>
     <row r="5" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="136"/>
-      <c r="C5" s="141"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="139"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="45"/>
@@ -6432,8 +6461,8 @@
       <c r="AK5" s="35"/>
     </row>
     <row r="6" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="136"/>
-      <c r="C6" s="141" t="s">
+      <c r="B6" s="138"/>
+      <c r="C6" s="139" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="35"/>
@@ -6472,8 +6501,8 @@
       <c r="AK6" s="49"/>
     </row>
     <row r="7" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="136"/>
-      <c r="C7" s="141"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="139"/>
       <c r="D7" s="35"/>
       <c r="E7" s="35"/>
       <c r="F7" s="45"/>
@@ -6510,8 +6539,8 @@
       <c r="AK7" s="35"/>
     </row>
     <row r="8" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="136"/>
-      <c r="C8" s="141" t="s">
+      <c r="B8" s="138"/>
+      <c r="C8" s="139" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="49"/>
@@ -6550,8 +6579,8 @@
       <c r="AK8" s="49"/>
     </row>
     <row r="9" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="136"/>
-      <c r="C9" s="141"/>
+      <c r="B9" s="138"/>
+      <c r="C9" s="139"/>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
       <c r="F9" s="43"/>
@@ -6588,8 +6617,8 @@
       <c r="AK9" s="35"/>
     </row>
     <row r="10" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="136"/>
-      <c r="C10" s="141" t="s">
+      <c r="B10" s="138"/>
+      <c r="C10" s="139" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="35"/>
@@ -6628,8 +6657,8 @@
       <c r="AK10" s="35"/>
     </row>
     <row r="11" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="136"/>
-      <c r="C11" s="141"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
       <c r="F11" s="43"/>
@@ -6666,8 +6695,8 @@
       <c r="AK11" s="35"/>
     </row>
     <row r="12" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="136"/>
-      <c r="C12" s="141" t="s">
+      <c r="B12" s="138"/>
+      <c r="C12" s="139" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="35"/>
@@ -6706,8 +6735,8 @@
       <c r="AK12" s="49"/>
     </row>
     <row r="13" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="136"/>
-      <c r="C13" s="141"/>
+      <c r="B13" s="138"/>
+      <c r="C13" s="139"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
       <c r="F13" s="43"/>
@@ -6744,10 +6773,10 @@
       <c r="AK13" s="35"/>
     </row>
     <row r="14" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="140" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="141" t="s">
         <v>77</v>
       </c>
       <c r="D14" s="49"/>
@@ -6786,8 +6815,8 @@
       <c r="AK14" s="51"/>
     </row>
     <row r="15" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="138"/>
-      <c r="C15" s="139"/>
+      <c r="B15" s="140"/>
+      <c r="C15" s="141"/>
       <c r="D15" s="51"/>
       <c r="E15" s="48"/>
       <c r="F15" s="45"/>
@@ -6824,8 +6853,8 @@
       <c r="AK15" s="51"/>
     </row>
     <row r="16" spans="2:47" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="138"/>
-      <c r="C16" s="139" t="s">
+      <c r="B16" s="140"/>
+      <c r="C16" s="141" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="49"/>
@@ -6864,8 +6893,8 @@
       <c r="AK16" s="51"/>
     </row>
     <row r="17" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="138"/>
-      <c r="C17" s="139"/>
+      <c r="B17" s="140"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="53"/>
       <c r="E17" s="48"/>
       <c r="F17" s="54"/>
@@ -6905,8 +6934,8 @@
       </c>
     </row>
     <row r="18" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="138"/>
-      <c r="C18" s="139" t="s">
+      <c r="B18" s="140"/>
+      <c r="C18" s="141" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="49"/>
@@ -6945,8 +6974,8 @@
       <c r="AK18" s="51"/>
     </row>
     <row r="19" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="138"/>
-      <c r="C19" s="139"/>
+      <c r="B19" s="140"/>
+      <c r="C19" s="141"/>
       <c r="D19" s="51"/>
       <c r="E19" s="48"/>
       <c r="F19" s="55"/>
@@ -6983,8 +7012,8 @@
       <c r="AK19" s="51"/>
     </row>
     <row r="20" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="138"/>
-      <c r="C20" s="139" t="s">
+      <c r="B20" s="140"/>
+      <c r="C20" s="141" t="s">
         <v>81</v>
       </c>
       <c r="D20" s="51"/>
@@ -7023,8 +7052,8 @@
       <c r="AK20" s="51"/>
     </row>
     <row r="21" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="138"/>
-      <c r="C21" s="139"/>
+      <c r="B21" s="140"/>
+      <c r="C21" s="141"/>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
       <c r="F21" s="54"/>
@@ -7061,8 +7090,8 @@
       <c r="AK21" s="51"/>
     </row>
     <row r="22" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="138"/>
-      <c r="C22" s="139" t="s">
+      <c r="B22" s="140"/>
+      <c r="C22" s="141" t="s">
         <v>82</v>
       </c>
       <c r="D22" s="51"/>
@@ -7101,8 +7130,8 @@
       <c r="AK22" s="51"/>
     </row>
     <row r="23" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="138"/>
-      <c r="C23" s="139"/>
+      <c r="B23" s="140"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
       <c r="F23" s="54"/>
@@ -7139,8 +7168,8 @@
       <c r="AK23" s="51"/>
     </row>
     <row r="24" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="138"/>
-      <c r="C24" s="139" t="s">
+      <c r="B24" s="140"/>
+      <c r="C24" s="141" t="s">
         <v>83</v>
       </c>
       <c r="D24" s="51"/>
@@ -7179,8 +7208,8 @@
       <c r="AK24" s="51"/>
     </row>
     <row r="25" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="138"/>
-      <c r="C25" s="139"/>
+      <c r="B25" s="140"/>
+      <c r="C25" s="141"/>
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
       <c r="F25" s="54"/>
@@ -7217,10 +7246,10 @@
       <c r="AK25" s="51"/>
     </row>
     <row r="26" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="141" t="s">
+      <c r="C26" s="139" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="35"/>
@@ -7259,8 +7288,8 @@
       <c r="AK26" s="35"/>
     </row>
     <row r="27" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="136"/>
-      <c r="C27" s="141"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="139"/>
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
       <c r="F27" s="43"/>
@@ -7297,8 +7326,8 @@
       <c r="AK27" s="35"/>
     </row>
     <row r="28" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="136"/>
-      <c r="C28" s="141" t="s">
+      <c r="B28" s="138"/>
+      <c r="C28" s="139" t="s">
         <v>86</v>
       </c>
       <c r="D28" s="35"/>
@@ -7337,15 +7366,15 @@
       <c r="AK28" s="35"/>
     </row>
     <row r="29" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="136"/>
-      <c r="C29" s="141"/>
+      <c r="B29" s="138"/>
+      <c r="C29" s="139"/>
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
       <c r="F29" s="43"/>
       <c r="G29" s="46"/>
       <c r="H29" s="47"/>
       <c r="I29" s="35"/>
-      <c r="J29" s="162"/>
+      <c r="J29" s="136"/>
       <c r="K29" s="35"/>
       <c r="L29" s="39"/>
       <c r="M29" s="35"/>
@@ -7375,8 +7404,8 @@
       <c r="AK29" s="35"/>
     </row>
     <row r="30" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="136"/>
-      <c r="C30" s="141" t="s">
+      <c r="B30" s="138"/>
+      <c r="C30" s="139" t="s">
         <v>87</v>
       </c>
       <c r="D30" s="35"/>
@@ -7415,17 +7444,17 @@
       <c r="AK30" s="35"/>
     </row>
     <row r="31" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="136"/>
-      <c r="C31" s="141"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="139"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
       <c r="F31" s="45"/>
       <c r="G31" s="46"/>
       <c r="H31" s="47"/>
       <c r="I31" s="35"/>
-      <c r="J31" s="162"/>
-      <c r="K31" s="162"/>
-      <c r="L31" s="39"/>
+      <c r="J31" s="136"/>
+      <c r="K31" s="136"/>
+      <c r="L31" s="165"/>
       <c r="M31" s="35"/>
       <c r="N31" s="40"/>
       <c r="O31" s="41"/>
@@ -7453,8 +7482,8 @@
       <c r="AK31" s="35"/>
     </row>
     <row r="32" spans="2:40" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="136"/>
-      <c r="C32" s="141" t="s">
+      <c r="B32" s="138"/>
+      <c r="C32" s="139" t="s">
         <v>88</v>
       </c>
       <c r="D32" s="35"/>
@@ -7493,8 +7522,8 @@
       <c r="AK32" s="35"/>
     </row>
     <row r="33" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="136"/>
-      <c r="C33" s="141"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="139"/>
       <c r="D33" s="35"/>
       <c r="E33" s="35"/>
       <c r="F33" s="43"/>
@@ -7531,10 +7560,10 @@
       <c r="AK33" s="35"/>
     </row>
     <row r="34" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="138" t="s">
+      <c r="B34" s="140" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="140" t="s">
+      <c r="C34" s="142" t="s">
         <v>90</v>
       </c>
       <c r="D34" s="51"/>
@@ -7573,8 +7602,8 @@
       <c r="AK34" s="51"/>
     </row>
     <row r="35" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="138"/>
-      <c r="C35" s="140"/>
+      <c r="B35" s="140"/>
+      <c r="C35" s="142"/>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
       <c r="F35" s="54"/>
@@ -7582,7 +7611,7 @@
       <c r="H35" s="50"/>
       <c r="I35" s="51"/>
       <c r="J35" s="51"/>
-      <c r="K35" s="163"/>
+      <c r="K35" s="137"/>
       <c r="L35" s="39"/>
       <c r="M35" s="51"/>
       <c r="N35" s="52"/>
@@ -7611,8 +7640,8 @@
       <c r="AK35" s="51"/>
     </row>
     <row r="36" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="138"/>
-      <c r="C36" s="140" t="s">
+      <c r="B36" s="140"/>
+      <c r="C36" s="142" t="s">
         <v>91</v>
       </c>
       <c r="D36" s="51"/>
@@ -7651,8 +7680,8 @@
       <c r="AK36" s="51"/>
     </row>
     <row r="37" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="138"/>
-      <c r="C37" s="140"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="142"/>
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="54"/>
@@ -7660,7 +7689,7 @@
       <c r="H37" s="50"/>
       <c r="I37" s="51"/>
       <c r="J37" s="51"/>
-      <c r="K37" s="163"/>
+      <c r="K37" s="137"/>
       <c r="L37" s="39"/>
       <c r="M37" s="51"/>
       <c r="N37" s="52"/>
@@ -7689,8 +7718,8 @@
       <c r="AK37" s="51"/>
     </row>
     <row r="38" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="138"/>
-      <c r="C38" s="140" t="s">
+      <c r="B38" s="140"/>
+      <c r="C38" s="142" t="s">
         <v>92</v>
       </c>
       <c r="D38" s="51"/>
@@ -7729,8 +7758,8 @@
       <c r="AK38" s="51"/>
     </row>
     <row r="39" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="138"/>
-      <c r="C39" s="140"/>
+      <c r="B39" s="140"/>
+      <c r="C39" s="142"/>
       <c r="D39" s="51"/>
       <c r="E39" s="51"/>
       <c r="F39" s="54"/>
@@ -7767,8 +7796,8 @@
       <c r="AK39" s="51"/>
     </row>
     <row r="40" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="138"/>
-      <c r="C40" s="140" t="s">
+      <c r="B40" s="140"/>
+      <c r="C40" s="142" t="s">
         <v>93</v>
       </c>
       <c r="D40" s="51"/>
@@ -7807,8 +7836,8 @@
       <c r="AK40" s="51"/>
     </row>
     <row r="41" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="138"/>
-      <c r="C41" s="140"/>
+      <c r="B41" s="140"/>
+      <c r="C41" s="142"/>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
       <c r="F41" s="54"/>
@@ -7845,10 +7874,10 @@
       <c r="AK41" s="51"/>
     </row>
     <row r="42" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="136" t="s">
+      <c r="B42" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="137" t="s">
+      <c r="C42" s="143" t="s">
         <v>94</v>
       </c>
       <c r="D42" s="35"/>
@@ -7887,8 +7916,8 @@
       <c r="AK42" s="35"/>
     </row>
     <row r="43" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="136"/>
-      <c r="C43" s="137"/>
+      <c r="B43" s="138"/>
+      <c r="C43" s="143"/>
       <c r="D43" s="35"/>
       <c r="E43" s="35"/>
       <c r="F43" s="43"/>
@@ -7925,8 +7954,8 @@
       <c r="AK43" s="35"/>
     </row>
     <row r="44" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="136"/>
-      <c r="C44" s="137" t="s">
+      <c r="B44" s="138"/>
+      <c r="C44" s="143" t="s">
         <v>95</v>
       </c>
       <c r="D44" s="35"/>
@@ -7965,8 +7994,8 @@
       <c r="AK44" s="35"/>
     </row>
     <row r="45" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="136"/>
-      <c r="C45" s="137"/>
+      <c r="B45" s="138"/>
+      <c r="C45" s="143"/>
       <c r="D45" s="35"/>
       <c r="E45" s="35"/>
       <c r="F45" s="43"/>
@@ -8003,10 +8032,10 @@
       <c r="AK45" s="35"/>
     </row>
     <row r="46" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="138" t="s">
+      <c r="B46" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="139" t="s">
+      <c r="C46" s="141" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="51"/>
@@ -8045,8 +8074,8 @@
       <c r="AK46" s="51"/>
     </row>
     <row r="47" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="138"/>
-      <c r="C47" s="139"/>
+      <c r="B47" s="140"/>
+      <c r="C47" s="141"/>
       <c r="D47" s="51"/>
       <c r="E47" s="51"/>
       <c r="F47" s="54"/>
@@ -8087,8 +8116,8 @@
       <c r="AO47" s="49"/>
     </row>
     <row r="48" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="138"/>
-      <c r="C48" s="139" t="s">
+      <c r="B48" s="140"/>
+      <c r="C48" s="141" t="s">
         <v>98</v>
       </c>
       <c r="D48" s="51"/>
@@ -8131,8 +8160,8 @@
       <c r="AO48" s="48"/>
     </row>
     <row r="49" spans="2:41" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="138"/>
-      <c r="C49" s="139"/>
+      <c r="B49" s="140"/>
+      <c r="C49" s="141"/>
       <c r="D49" s="51"/>
       <c r="E49" s="51"/>
       <c r="F49" s="54"/>
@@ -8174,6 +8203,29 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B26:B33"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
@@ -8181,29 +8233,6 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B26:B33"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="C48:C49"/>
   </mergeCells>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape"/>
@@ -8236,10 +8265,10 @@
       <c r="B1" s="58"/>
     </row>
     <row r="2" spans="2:30" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="144" t="s">
+      <c r="C2" s="148" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="59" t="s">
@@ -8248,33 +8277,33 @@
       <c r="E2" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="157" t="s">
+      <c r="F2" s="144" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="161"/>
-      <c r="J2" s="157" t="s">
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="144" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="157"/>
-      <c r="L2" s="157"/>
-      <c r="M2" s="161"/>
-      <c r="N2" s="157" t="s">
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="144" t="s">
         <v>105</v>
       </c>
-      <c r="O2" s="157"/>
-      <c r="P2" s="157"/>
-      <c r="Q2" s="161"/>
-      <c r="R2" s="157" t="s">
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
+      <c r="Q2" s="156"/>
+      <c r="R2" s="144" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="158"/>
+      <c r="S2" s="145"/>
       <c r="AD2" s="17"/>
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B3" s="160"/>
-      <c r="C3" s="147"/>
+      <c r="B3" s="154"/>
+      <c r="C3" s="155"/>
       <c r="D3" s="61" t="s">
         <v>107</v>
       </c>
@@ -8328,10 +8357,10 @@
       </c>
     </row>
     <row r="4" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="146" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="148" t="s">
         <v>110</v>
       </c>
       <c r="D4" s="66"/>
@@ -8355,8 +8384,8 @@
       </c>
     </row>
     <row r="5" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="143"/>
-      <c r="C5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="149"/>
       <c r="D5" s="72"/>
       <c r="E5" s="73"/>
       <c r="F5" s="74"/>
@@ -8375,8 +8404,8 @@
       <c r="S5" s="78"/>
     </row>
     <row r="6" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="143"/>
-      <c r="C6" s="146" t="s">
+      <c r="B6" s="146"/>
+      <c r="C6" s="150" t="s">
         <v>112</v>
       </c>
       <c r="D6" s="79"/>
@@ -8395,14 +8424,14 @@
       <c r="Q6" s="80"/>
       <c r="R6" s="84"/>
       <c r="S6" s="85"/>
-      <c r="U6" s="159" t="s">
+      <c r="U6" s="151" t="s">
         <v>113</v>
       </c>
-      <c r="V6" s="159"/>
+      <c r="V6" s="151"/>
     </row>
     <row r="7" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="143"/>
-      <c r="C7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="149"/>
       <c r="D7" s="72"/>
       <c r="E7" s="73"/>
       <c r="F7" s="77"/>
@@ -8424,8 +8453,8 @@
       </c>
     </row>
     <row r="8" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="143"/>
-      <c r="C8" s="146" t="s">
+      <c r="B8" s="146"/>
+      <c r="C8" s="150" t="s">
         <v>115</v>
       </c>
       <c r="D8" s="79"/>
@@ -8449,8 +8478,8 @@
       </c>
     </row>
     <row r="9" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="143"/>
-      <c r="C9" s="145"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="149"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="77"/>
@@ -8469,8 +8498,8 @@
       <c r="S9" s="78"/>
     </row>
     <row r="10" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="143"/>
-      <c r="C10" s="146" t="s">
+      <c r="B10" s="146"/>
+      <c r="C10" s="150" t="s">
         <v>117</v>
       </c>
       <c r="D10" s="79"/>
@@ -8491,8 +8520,8 @@
       <c r="S10" s="85"/>
     </row>
     <row r="11" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="155"/>
-      <c r="C11" s="156"/>
+      <c r="B11" s="147"/>
+      <c r="C11" s="152"/>
       <c r="D11" s="86"/>
       <c r="E11" s="87"/>
       <c r="F11" s="88"/>
@@ -8511,10 +8540,10 @@
       <c r="S11" s="91"/>
     </row>
     <row r="12" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="154" t="s">
+      <c r="B12" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="144" t="s">
+      <c r="C12" s="148" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="66"/>
@@ -8535,8 +8564,8 @@
       <c r="S12" s="71"/>
     </row>
     <row r="13" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="143"/>
-      <c r="C13" s="145"/>
+      <c r="B13" s="146"/>
+      <c r="C13" s="149"/>
       <c r="D13" s="72"/>
       <c r="E13" s="73"/>
       <c r="F13" s="77"/>
@@ -8555,8 +8584,8 @@
       <c r="S13" s="78"/>
     </row>
     <row r="14" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="143"/>
-      <c r="C14" s="146" t="s">
+      <c r="B14" s="146"/>
+      <c r="C14" s="150" t="s">
         <v>120</v>
       </c>
       <c r="D14" s="94"/>
@@ -8577,8 +8606,8 @@
       <c r="S14" s="85"/>
     </row>
     <row r="15" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="143"/>
-      <c r="C15" s="145"/>
+      <c r="B15" s="146"/>
+      <c r="C15" s="149"/>
       <c r="D15" s="72"/>
       <c r="E15" s="73"/>
       <c r="F15" s="77"/>
@@ -8597,8 +8626,8 @@
       <c r="S15" s="78"/>
     </row>
     <row r="16" spans="2:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="143"/>
-      <c r="C16" s="146" t="s">
+      <c r="B16" s="146"/>
+      <c r="C16" s="150" t="s">
         <v>121</v>
       </c>
       <c r="D16" s="79"/>
@@ -8619,8 +8648,8 @@
       <c r="S16" s="85"/>
     </row>
     <row r="17" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="155"/>
-      <c r="C17" s="156"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="152"/>
       <c r="D17" s="86"/>
       <c r="E17" s="87"/>
       <c r="F17" s="88"/>
@@ -8639,10 +8668,10 @@
       <c r="S17" s="91"/>
     </row>
     <row r="18" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="157" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="144" t="s">
+      <c r="C18" s="148" t="s">
         <v>123</v>
       </c>
       <c r="D18" s="66"/>
@@ -8663,8 +8692,8 @@
       <c r="S18" s="71"/>
     </row>
     <row r="19" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="143"/>
-      <c r="C19" s="145"/>
+      <c r="B19" s="146"/>
+      <c r="C19" s="149"/>
       <c r="D19" s="72"/>
       <c r="E19" s="73"/>
       <c r="F19" s="77"/>
@@ -8683,8 +8712,8 @@
       <c r="S19" s="78"/>
     </row>
     <row r="20" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="143"/>
-      <c r="C20" s="146" t="s">
+      <c r="B20" s="146"/>
+      <c r="C20" s="150" t="s">
         <v>124</v>
       </c>
       <c r="D20" s="79"/>
@@ -8705,8 +8734,8 @@
       <c r="S20" s="85"/>
     </row>
     <row r="21" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="143"/>
-      <c r="C21" s="145"/>
+      <c r="B21" s="146"/>
+      <c r="C21" s="149"/>
       <c r="D21" s="72"/>
       <c r="E21" s="73"/>
       <c r="F21" s="77"/>
@@ -8725,8 +8754,8 @@
       <c r="S21" s="78"/>
     </row>
     <row r="22" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="143"/>
-      <c r="C22" s="146" t="s">
+      <c r="B22" s="146"/>
+      <c r="C22" s="150" t="s">
         <v>125</v>
       </c>
       <c r="D22" s="79"/>
@@ -8747,8 +8776,8 @@
       <c r="S22" s="85"/>
     </row>
     <row r="23" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="155"/>
-      <c r="C23" s="156"/>
+      <c r="B23" s="147"/>
+      <c r="C23" s="152"/>
       <c r="D23" s="86"/>
       <c r="E23" s="87"/>
       <c r="F23" s="88"/>
@@ -8767,10 +8796,10 @@
       <c r="S23" s="91"/>
     </row>
     <row r="24" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="142" t="s">
+      <c r="B24" s="157" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="144" t="s">
+      <c r="C24" s="148" t="s">
         <v>127</v>
       </c>
       <c r="D24" s="66"/>
@@ -8791,8 +8820,8 @@
       <c r="S24" s="71"/>
     </row>
     <row r="25" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="143"/>
-      <c r="C25" s="145"/>
+      <c r="B25" s="146"/>
+      <c r="C25" s="149"/>
       <c r="D25" s="72"/>
       <c r="E25" s="73"/>
       <c r="F25" s="77"/>
@@ -8811,8 +8840,8 @@
       <c r="S25" s="78"/>
     </row>
     <row r="26" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="143"/>
-      <c r="C26" s="146" t="s">
+      <c r="B26" s="146"/>
+      <c r="C26" s="150" t="s">
         <v>128</v>
       </c>
       <c r="D26" s="79"/>
@@ -8833,8 +8862,8 @@
       <c r="S26" s="85"/>
     </row>
     <row r="27" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="143"/>
-      <c r="C27" s="145"/>
+      <c r="B27" s="146"/>
+      <c r="C27" s="149"/>
       <c r="D27" s="72"/>
       <c r="E27" s="73"/>
       <c r="F27" s="77"/>
@@ -8853,8 +8882,8 @@
       <c r="S27" s="78"/>
     </row>
     <row r="28" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="143"/>
-      <c r="C28" s="146" t="s">
+      <c r="B28" s="146"/>
+      <c r="C28" s="150" t="s">
         <v>129</v>
       </c>
       <c r="D28" s="79"/>
@@ -8875,8 +8904,8 @@
       <c r="S28" s="85"/>
     </row>
     <row r="29" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="143"/>
-      <c r="C29" s="147"/>
+      <c r="B29" s="146"/>
+      <c r="C29" s="155"/>
       <c r="D29" s="99"/>
       <c r="E29" s="100"/>
       <c r="F29" s="101"/>
@@ -8895,10 +8924,10 @@
       <c r="S29" s="105"/>
     </row>
     <row r="30" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="151" t="s">
+      <c r="C30" s="161" t="s">
         <v>73</v>
       </c>
       <c r="D30" s="66"/>
@@ -8919,8 +8948,8 @@
       <c r="S30" s="110"/>
     </row>
     <row r="31" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="149"/>
-      <c r="C31" s="152"/>
+      <c r="B31" s="159"/>
+      <c r="C31" s="162"/>
       <c r="D31" s="72"/>
       <c r="E31" s="111"/>
       <c r="F31" s="112"/>
@@ -8939,8 +8968,8 @@
       <c r="S31" s="78"/>
     </row>
     <row r="32" spans="2:19" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="149"/>
-      <c r="C32" s="152" t="s">
+      <c r="B32" s="159"/>
+      <c r="C32" s="162" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="79"/>
@@ -8961,8 +8990,8 @@
       <c r="S32" s="120"/>
     </row>
     <row r="33" spans="2:22" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="149"/>
-      <c r="C33" s="152"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="162"/>
       <c r="D33" s="72"/>
       <c r="E33" s="111"/>
       <c r="F33" s="115"/>
@@ -8981,8 +9010,8 @@
       <c r="S33" s="78"/>
     </row>
     <row r="34" spans="2:22" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="149"/>
-      <c r="C34" s="145" t="s">
+      <c r="B34" s="159"/>
+      <c r="C34" s="149" t="s">
         <v>130</v>
       </c>
       <c r="D34" s="99"/>
@@ -9007,8 +9036,8 @@
       </c>
     </row>
     <row r="35" spans="2:22" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="150"/>
-      <c r="C35" s="153"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="163"/>
       <c r="D35" s="86"/>
       <c r="E35" s="130"/>
       <c r="F35" s="131"/>
@@ -9032,6 +9061,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="B4:B11"/>
     <mergeCell ref="C4:C5"/>
@@ -9044,22 +9089,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>